<commit_message>
1) created new R-script for SCFA-data 2) SPI-file: still need to adjust STdev in Cohens calculations 3) created Samplesize-file
</commit_message>
<xml_diff>
--- a/SGPI_All_Donors.xlsx
+++ b/SGPI_All_Donors.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lmmiclot\OneDrive - UGent\PhD\Experiments\2017_8 - Batch effect MO\General_Results\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lmmiclot\OneDrive - UGent\PhD\Experiments\2017_8 - Batch effect MO\20180515_Illumina\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9192" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9192"/>
   </bookViews>
   <sheets>
     <sheet name="Overview_Cellcounts" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
   </definedNames>
   <calcPr calcId="162913"/>
   <pivotCaches>
-    <pivotCache cacheId="1" r:id="rId3"/>
+    <pivotCache cacheId="6" r:id="rId3"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -97,8 +97,11 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <numFmts count="1">
+  <numFmts count="4">
     <numFmt numFmtId="164" formatCode="0.0"/>
+    <numFmt numFmtId="165" formatCode="0.000"/>
+    <numFmt numFmtId="166" formatCode="0.0000"/>
+    <numFmt numFmtId="167" formatCode="0.00000"/>
   </numFmts>
   <fonts count="6" x14ac:knownFonts="1">
     <font>
@@ -144,7 +147,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -154,6 +157,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -180,7 +189,7 @@
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -220,13 +229,85 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Good" xfId="2" builtinId="26"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
-  <dxfs count="7">
+  <dxfs count="29">
+    <dxf>
+      <numFmt numFmtId="165" formatCode="0.000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="165" formatCode="0.000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="1" formatCode="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="1" formatCode="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="167" formatCode="0.00000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="166" formatCode="0.0000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="165" formatCode="0.000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="170" formatCode="0.00000000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="169" formatCode="0.0000000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="168" formatCode="0.000000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="167" formatCode="0.00000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="166" formatCode="0.0000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="165" formatCode="0.000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
     <dxf>
       <numFmt numFmtId="2" formatCode="0.00"/>
     </dxf>
@@ -262,7 +343,7 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" refreshedBy="Lisa Miclotte" refreshedDate="43203.546567013887" createdVersion="6" refreshedVersion="6" minRefreshableVersion="3" recordCount="420">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" refreshedBy="Lisa Miclotte" refreshedDate="43250.362251388891" createdVersion="6" refreshedVersion="6" minRefreshableVersion="3" recordCount="420">
   <cacheSource type="worksheet">
     <worksheetSource ref="A1:G421" sheet="Overview_Cellcounts"/>
   </cacheSource>
@@ -292,15 +373,7 @@
       </sharedItems>
     </cacheField>
     <cacheField name="Donor" numFmtId="0">
-      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="1" maxValue="7" count="7">
-        <n v="1"/>
-        <n v="2"/>
-        <n v="3"/>
-        <n v="4"/>
-        <n v="5"/>
-        <n v="6"/>
-        <n v="7"/>
-      </sharedItems>
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="1" maxValue="7"/>
     </cacheField>
     <cacheField name="Live_Count" numFmtId="2">
       <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="7.6020599913279625" maxValue="10.050804808616556"/>
@@ -326,7 +399,7 @@
     <x v="0"/>
     <x v="0"/>
     <x v="0"/>
-    <x v="0"/>
+    <n v="1"/>
     <n v="9.4240098632701716"/>
     <n v="9.7959954431166096"/>
     <n v="0.96202677083646226"/>
@@ -335,7 +408,7 @@
     <x v="0"/>
     <x v="1"/>
     <x v="0"/>
-    <x v="0"/>
+    <n v="1"/>
     <n v="9.5088065209152948"/>
     <n v="9.71093626081195"/>
     <n v="0.97918534995308937"/>
@@ -344,7 +417,7 @@
     <x v="0"/>
     <x v="2"/>
     <x v="0"/>
-    <x v="0"/>
+    <n v="1"/>
     <n v="9.3935803223956835"/>
     <n v="9.7518996874222506"/>
     <n v="0.96325645499730495"/>
@@ -353,7 +426,7 @@
     <x v="0"/>
     <x v="3"/>
     <x v="0"/>
-    <x v="0"/>
+    <n v="1"/>
     <n v="9.251318383953441"/>
     <n v="9.7589590804382453"/>
     <n v="0.94798208576339194"/>
@@ -362,7 +435,7 @@
     <x v="1"/>
     <x v="0"/>
     <x v="0"/>
-    <x v="0"/>
+    <n v="1"/>
     <n v="9.3311163808053248"/>
     <n v="9.8003202707418868"/>
     <n v="0.95212361668043288"/>
@@ -371,7 +444,7 @@
     <x v="1"/>
     <x v="1"/>
     <x v="0"/>
-    <x v="0"/>
+    <n v="1"/>
     <n v="9.4477477055885029"/>
     <n v="9.7634354841728648"/>
     <n v="0.96766632205476122"/>
@@ -380,7 +453,7 @@
     <x v="1"/>
     <x v="2"/>
     <x v="0"/>
-    <x v="0"/>
+    <n v="1"/>
     <n v="9.6001217007287352"/>
     <n v="9.8325254861957845"/>
     <n v="0.9763637749230013"/>
@@ -389,7 +462,7 @@
     <x v="1"/>
     <x v="3"/>
     <x v="0"/>
-    <x v="0"/>
+    <n v="1"/>
     <n v="9.251318383953441"/>
     <n v="9.7589590804382453"/>
     <n v="0.94798208576339194"/>
@@ -398,7 +471,7 @@
     <x v="2"/>
     <x v="0"/>
     <x v="0"/>
-    <x v="0"/>
+    <n v="1"/>
     <n v="9.2684762698640881"/>
     <n v="9.8419553938948123"/>
     <n v="0.94173118033165781"/>
@@ -407,7 +480,7 @@
     <x v="2"/>
     <x v="1"/>
     <x v="0"/>
-    <x v="0"/>
+    <n v="1"/>
     <n v="9.3866328741010463"/>
     <n v="9.7635026093269897"/>
     <n v="0.96140015009921509"/>
@@ -416,7 +489,7 @@
     <x v="2"/>
     <x v="2"/>
     <x v="0"/>
-    <x v="0"/>
+    <n v="1"/>
     <n v="9.3753785433333565"/>
     <n v="9.8360597390209517"/>
     <n v="0.95316405065536436"/>
@@ -425,7 +498,7 @@
     <x v="2"/>
     <x v="3"/>
     <x v="0"/>
-    <x v="0"/>
+    <n v="1"/>
     <n v="9.251318383953441"/>
     <n v="9.7589590804382453"/>
     <n v="0.94798208576339194"/>
@@ -434,7 +507,7 @@
     <x v="3"/>
     <x v="0"/>
     <x v="0"/>
-    <x v="0"/>
+    <n v="1"/>
     <n v="9.2926549660873778"/>
     <n v="9.7513091228089159"/>
     <n v="0.95296486338960196"/>
@@ -443,7 +516,7 @@
     <x v="3"/>
     <x v="1"/>
     <x v="0"/>
-    <x v="0"/>
+    <n v="1"/>
     <n v="9.1502446512516684"/>
     <n v="9.8269044061909163"/>
     <n v="0.93114212503044658"/>
@@ -452,7 +525,7 @@
     <x v="3"/>
     <x v="2"/>
     <x v="0"/>
-    <x v="0"/>
+    <n v="1"/>
     <n v="8.7388714951670927"/>
     <n v="9.8245504015026643"/>
     <n v="0.88949327328306882"/>
@@ -461,7 +534,7 @@
     <x v="3"/>
     <x v="3"/>
     <x v="0"/>
-    <x v="0"/>
+    <n v="1"/>
     <n v="9.251318383953441"/>
     <n v="9.7589590804382453"/>
     <n v="0.94798208576339194"/>
@@ -470,7 +543,7 @@
     <x v="4"/>
     <x v="0"/>
     <x v="0"/>
-    <x v="0"/>
+    <n v="1"/>
     <n v="9.2630141721297949"/>
     <n v="9.8023631994928646"/>
     <n v="0.94497765320601734"/>
@@ -479,7 +552,7 @@
     <x v="4"/>
     <x v="1"/>
     <x v="0"/>
-    <x v="0"/>
+    <n v="1"/>
     <n v="8.9744354014395178"/>
     <n v="9.8607583110976247"/>
     <n v="0.91011615114218858"/>
@@ -488,7 +561,7 @@
     <x v="4"/>
     <x v="2"/>
     <x v="0"/>
-    <x v="0"/>
+    <n v="1"/>
     <n v="8.5061713132926293"/>
     <n v="9.8690321730233617"/>
     <n v="0.86190531798487169"/>
@@ -497,7 +570,7 @@
     <x v="4"/>
     <x v="3"/>
     <x v="0"/>
-    <x v="0"/>
+    <n v="1"/>
     <n v="9.251318383953441"/>
     <n v="9.7589590804382453"/>
     <n v="0.94798208576339194"/>
@@ -506,7 +579,7 @@
     <x v="0"/>
     <x v="0"/>
     <x v="1"/>
-    <x v="0"/>
+    <n v="1"/>
     <n v="9.2054729293438875"/>
     <n v="9.5807438955437263"/>
     <n v="0.96083070685415273"/>
@@ -515,7 +588,7 @@
     <x v="0"/>
     <x v="1"/>
     <x v="1"/>
-    <x v="0"/>
+    <n v="1"/>
     <n v="9.1672268755754658"/>
     <n v="9.4961441768985466"/>
     <n v="0.96536306787303794"/>
@@ -524,7 +597,7 @@
     <x v="0"/>
     <x v="2"/>
     <x v="1"/>
-    <x v="0"/>
+    <n v="1"/>
     <n v="9.2354990848304368"/>
     <n v="9.540024483789427"/>
     <n v="0.96807918056432196"/>
@@ -533,7 +606,7 @@
     <x v="0"/>
     <x v="3"/>
     <x v="1"/>
-    <x v="0"/>
+    <n v="1"/>
     <n v="9.168729630645327"/>
     <n v="9.5458334787978423"/>
     <n v="0.96049545081735432"/>
@@ -542,7 +615,7 @@
     <x v="1"/>
     <x v="0"/>
     <x v="1"/>
-    <x v="0"/>
+    <n v="1"/>
     <n v="9.1595530296548873"/>
     <n v="9.5195880421880208"/>
     <n v="0.96217955956312773"/>
@@ -551,7 +624,7 @@
     <x v="1"/>
     <x v="1"/>
     <x v="1"/>
-    <x v="0"/>
+    <n v="1"/>
     <n v="9.0892006707668784"/>
     <n v="9.3440318484731719"/>
     <n v="0.97272792068362512"/>
@@ -560,7 +633,7 @@
     <x v="1"/>
     <x v="2"/>
     <x v="1"/>
-    <x v="0"/>
+    <n v="1"/>
     <n v="9.1945830421822663"/>
     <n v="9.5510452627559186"/>
     <n v="0.96267819795979104"/>
@@ -569,7 +642,7 @@
     <x v="1"/>
     <x v="3"/>
     <x v="1"/>
-    <x v="0"/>
+    <n v="1"/>
     <n v="9.168729630645327"/>
     <n v="9.5458334787978423"/>
     <n v="0.96049545081735432"/>
@@ -578,7 +651,7 @@
     <x v="2"/>
     <x v="0"/>
     <x v="1"/>
-    <x v="0"/>
+    <n v="1"/>
     <n v="9.1105766609773529"/>
     <n v="9.5380287978814131"/>
     <n v="0.95518443632724137"/>
@@ -587,7 +660,7 @@
     <x v="2"/>
     <x v="1"/>
     <x v="1"/>
-    <x v="0"/>
+    <n v="1"/>
     <n v="9.153212513775344"/>
     <n v="9.5569716761534185"/>
     <n v="0.95775239520845967"/>
@@ -596,7 +669,7 @@
     <x v="2"/>
     <x v="2"/>
     <x v="1"/>
-    <x v="0"/>
+    <n v="1"/>
     <n v="9.0472355643208218"/>
     <n v="9.5537745648723433"/>
     <n v="0.94698022262174975"/>
@@ -605,7 +678,7 @@
     <x v="2"/>
     <x v="3"/>
     <x v="1"/>
-    <x v="0"/>
+    <n v="1"/>
     <n v="9.168729630645327"/>
     <n v="9.5458334787978423"/>
     <n v="0.96049545081735432"/>
@@ -614,7 +687,7 @@
     <x v="3"/>
     <x v="0"/>
     <x v="1"/>
-    <x v="0"/>
+    <n v="1"/>
     <n v="9.1901056208558032"/>
     <n v="9.5266352833406884"/>
     <n v="0.96467486657399626"/>
@@ -623,7 +696,7 @@
     <x v="3"/>
     <x v="1"/>
     <x v="1"/>
-    <x v="0"/>
+    <n v="1"/>
     <n v="9.1333509834420443"/>
     <n v="9.5368041942281039"/>
     <n v="0.95769513533367512"/>
@@ -632,7 +705,7 @@
     <x v="3"/>
     <x v="2"/>
     <x v="1"/>
-    <x v="0"/>
+    <n v="1"/>
     <n v="8.8222192947339195"/>
     <n v="9.3550163495328782"/>
     <n v="0.94304691356038484"/>
@@ -641,7 +714,7 @@
     <x v="3"/>
     <x v="3"/>
     <x v="1"/>
-    <x v="0"/>
+    <n v="1"/>
     <n v="9.168729630645327"/>
     <n v="9.5458334787978423"/>
     <n v="0.96049545081735432"/>
@@ -650,7 +723,7 @@
     <x v="4"/>
     <x v="0"/>
     <x v="1"/>
-    <x v="0"/>
+    <n v="1"/>
     <n v="9.0873205963302244"/>
     <n v="9.5530614370033273"/>
     <n v="0.95124695431465789"/>
@@ -659,7 +732,7 @@
     <x v="4"/>
     <x v="1"/>
     <x v="1"/>
-    <x v="0"/>
+    <n v="1"/>
     <n v="9.0857169504715038"/>
     <n v="9.6471008003473742"/>
     <n v="0.94180802486736159"/>
@@ -668,7 +741,7 @@
     <x v="4"/>
     <x v="2"/>
     <x v="1"/>
-    <x v="0"/>
+    <n v="1"/>
     <n v="8.2898917983084051"/>
     <n v="9.4268491058880883"/>
     <n v="0.87939158728344025"/>
@@ -677,7 +750,7 @@
     <x v="4"/>
     <x v="3"/>
     <x v="1"/>
-    <x v="0"/>
+    <n v="1"/>
     <n v="9.168729630645327"/>
     <n v="9.5458334787978423"/>
     <n v="0.96049545081735432"/>
@@ -686,7 +759,7 @@
     <x v="0"/>
     <x v="0"/>
     <x v="2"/>
-    <x v="0"/>
+    <n v="1"/>
     <n v="9.0140822097122353"/>
     <n v="9.7329144076787184"/>
     <n v="0.92614419814486759"/>
@@ -695,7 +768,7 @@
     <x v="0"/>
     <x v="1"/>
     <x v="2"/>
-    <x v="0"/>
+    <n v="1"/>
     <n v="8.9746950033224557"/>
     <n v="9.5643288502157073"/>
     <n v="0.93835073468014918"/>
@@ -704,7 +777,7 @@
     <x v="0"/>
     <x v="2"/>
     <x v="2"/>
-    <x v="0"/>
+    <n v="1"/>
     <n v="9.0809833081820379"/>
     <n v="9.7188118714985308"/>
     <n v="0.93437175533904571"/>
@@ -713,7 +786,7 @@
     <x v="0"/>
     <x v="3"/>
     <x v="2"/>
-    <x v="0"/>
+    <n v="1"/>
     <n v="8.9865639267998496"/>
     <n v="9.8055269150509581"/>
     <n v="0.91647945129862995"/>
@@ -722,7 +795,7 @@
     <x v="1"/>
     <x v="0"/>
     <x v="2"/>
-    <x v="0"/>
+    <n v="1"/>
     <n v="9.0049378168560814"/>
     <n v="9.7776077025630368"/>
     <n v="0.92097556895185995"/>
@@ -731,7 +804,7 @@
     <x v="1"/>
     <x v="1"/>
     <x v="2"/>
-    <x v="0"/>
+    <n v="1"/>
     <n v="9.0756849251237313"/>
     <n v="9.7402908934145849"/>
     <n v="0.93176733882350538"/>
@@ -740,7 +813,7 @@
     <x v="1"/>
     <x v="2"/>
     <x v="2"/>
-    <x v="0"/>
+    <n v="1"/>
     <n v="9.0529253371925726"/>
     <n v="9.6746970504719343"/>
     <n v="0.93573217744848858"/>
@@ -749,7 +822,7 @@
     <x v="1"/>
     <x v="3"/>
     <x v="2"/>
-    <x v="0"/>
+    <n v="1"/>
     <n v="8.9865639267998496"/>
     <n v="9.8055269150509581"/>
     <n v="0.91647945129862995"/>
@@ -758,7 +831,7 @@
     <x v="2"/>
     <x v="0"/>
     <x v="2"/>
-    <x v="0"/>
+    <n v="1"/>
     <n v="8.9888618026444238"/>
     <n v="9.7626001736765815"/>
     <n v="0.92074464207615203"/>
@@ -767,7 +840,7 @@
     <x v="2"/>
     <x v="1"/>
     <x v="2"/>
-    <x v="0"/>
+    <n v="1"/>
     <n v="9.029213012228503"/>
     <n v="9.7609872359936976"/>
     <n v="0.92503071604614207"/>
@@ -776,7 +849,7 @@
     <x v="2"/>
     <x v="2"/>
     <x v="2"/>
-    <x v="0"/>
+    <n v="1"/>
     <n v="8.9542425094393252"/>
     <n v="9.7923521429554921"/>
     <n v="0.91441181635618629"/>
@@ -785,7 +858,7 @@
     <x v="2"/>
     <x v="3"/>
     <x v="2"/>
-    <x v="0"/>
+    <n v="1"/>
     <n v="8.9865639267998496"/>
     <n v="9.8055269150509581"/>
     <n v="0.91647945129862995"/>
@@ -794,7 +867,7 @@
     <x v="3"/>
     <x v="0"/>
     <x v="2"/>
-    <x v="0"/>
+    <n v="1"/>
     <n v="8.9286662482156345"/>
     <n v="9.639685159089554"/>
     <n v="0.92624044259334781"/>
@@ -803,7 +876,7 @@
     <x v="3"/>
     <x v="1"/>
     <x v="2"/>
-    <x v="0"/>
+    <n v="1"/>
     <n v="8.962139643030941"/>
     <n v="9.715279384761379"/>
     <n v="0.92247883854871393"/>
@@ -812,7 +885,7 @@
     <x v="3"/>
     <x v="2"/>
     <x v="2"/>
-    <x v="0"/>
+    <n v="1"/>
     <n v="8.9146518864155126"/>
     <n v="9.6231507885858463"/>
     <n v="0.92637557929460135"/>
@@ -821,7 +894,7 @@
     <x v="3"/>
     <x v="3"/>
     <x v="2"/>
-    <x v="0"/>
+    <n v="1"/>
     <n v="8.9865639267998496"/>
     <n v="9.8055269150509581"/>
     <n v="0.91647945129862995"/>
@@ -830,7 +903,7 @@
     <x v="4"/>
     <x v="0"/>
     <x v="2"/>
-    <x v="0"/>
+    <n v="1"/>
     <n v="8.8546349804879156"/>
     <n v="9.857332496431269"/>
     <n v="0.89827902058631293"/>
@@ -839,7 +912,7 @@
     <x v="4"/>
     <x v="1"/>
     <x v="2"/>
-    <x v="0"/>
+    <n v="1"/>
     <n v="8.6662192299578038"/>
     <n v="9.7003121608308831"/>
     <n v="0.89339591203583457"/>
@@ -848,7 +921,7 @@
     <x v="4"/>
     <x v="2"/>
     <x v="2"/>
-    <x v="0"/>
+    <n v="1"/>
     <n v="8.3890756251918219"/>
     <n v="9.6696263170163501"/>
     <n v="0.86756978503181148"/>
@@ -857,7 +930,7 @@
     <x v="4"/>
     <x v="3"/>
     <x v="2"/>
-    <x v="0"/>
+    <n v="1"/>
     <n v="8.9865639267998496"/>
     <n v="9.8055269150509581"/>
     <n v="0.91647945129862995"/>
@@ -866,7 +939,7 @@
     <x v="0"/>
     <x v="0"/>
     <x v="0"/>
-    <x v="1"/>
+    <n v="2"/>
     <n v="9.7556073505681944"/>
     <n v="9.2007002703907723"/>
     <n v="1.0603113962926491"/>
@@ -875,7 +948,7 @@
     <x v="0"/>
     <x v="1"/>
     <x v="0"/>
-    <x v="1"/>
+    <n v="2"/>
     <n v="9.7652023132964132"/>
     <n v="9.1735673914550091"/>
     <n v="1.0644934404027488"/>
@@ -884,7 +957,7 @@
     <x v="0"/>
     <x v="2"/>
     <x v="0"/>
-    <x v="1"/>
+    <n v="2"/>
     <n v="9.7614502297307908"/>
     <n v="9.2142293867577898"/>
     <n v="1.0593886715865179"/>
@@ -893,7 +966,7 @@
     <x v="0"/>
     <x v="3"/>
     <x v="0"/>
-    <x v="1"/>
+    <n v="2"/>
     <n v="9.6928388782593551"/>
     <n v="9.188288478528257"/>
     <n v="1.054912337690546"/>
@@ -902,7 +975,7 @@
     <x v="1"/>
     <x v="0"/>
     <x v="0"/>
-    <x v="1"/>
+    <n v="2"/>
     <n v="9.7192498325707817"/>
     <n v="9.1055233048658941"/>
     <n v="1.0674015657482221"/>
@@ -911,7 +984,7 @@
     <x v="1"/>
     <x v="1"/>
     <x v="0"/>
-    <x v="1"/>
+    <n v="2"/>
     <n v="9.7343684796821677"/>
     <n v="9.2425471882742229"/>
     <n v="1.0532127433476246"/>
@@ -920,7 +993,7 @@
     <x v="1"/>
     <x v="2"/>
     <x v="0"/>
-    <x v="1"/>
+    <n v="2"/>
     <n v="9.6648006241782589"/>
     <n v="9.2698516194739131"/>
     <n v="1.0426057525963679"/>
@@ -929,7 +1002,7 @@
     <x v="1"/>
     <x v="3"/>
     <x v="0"/>
-    <x v="1"/>
+    <n v="2"/>
     <n v="9.6928388782593551"/>
     <n v="9.188288478528257"/>
     <n v="1.054912337690546"/>
@@ -938,7 +1011,7 @@
     <x v="2"/>
     <x v="0"/>
     <x v="0"/>
-    <x v="1"/>
+    <n v="2"/>
     <n v="9.7320956853205001"/>
     <n v="9.288745899918613"/>
     <n v="1.0477297786136848"/>
@@ -947,7 +1020,7 @@
     <x v="2"/>
     <x v="1"/>
     <x v="0"/>
-    <x v="1"/>
+    <n v="2"/>
     <n v="9.7092169400401627"/>
     <n v="9.3651892342938226"/>
     <n v="1.0367347308356105"/>
@@ -956,7 +1029,7 @@
     <x v="2"/>
     <x v="2"/>
     <x v="0"/>
-    <x v="1"/>
+    <n v="2"/>
     <n v="9.5113172699720607"/>
     <n v="9.594562603462764"/>
     <n v="0.99132369687590982"/>
@@ -965,7 +1038,7 @@
     <x v="2"/>
     <x v="3"/>
     <x v="0"/>
-    <x v="1"/>
+    <n v="2"/>
     <n v="9.6928388782593551"/>
     <n v="9.188288478528257"/>
     <n v="1.054912337690546"/>
@@ -974,7 +1047,7 @@
     <x v="3"/>
     <x v="0"/>
     <x v="0"/>
-    <x v="1"/>
+    <n v="2"/>
     <n v="9.7260849592677179"/>
     <n v="9.1717042969019289"/>
     <n v="1.0604446724861214"/>
@@ -983,7 +1056,7 @@
     <x v="3"/>
     <x v="1"/>
     <x v="0"/>
-    <x v="1"/>
+    <n v="2"/>
     <n v="9.3127076760772045"/>
     <n v="9.5661298447655234"/>
     <n v="0.97350839129295441"/>
@@ -992,7 +1065,7 @@
     <x v="3"/>
     <x v="2"/>
     <x v="0"/>
-    <x v="1"/>
+    <n v="2"/>
     <n v="8.9659830573640864"/>
     <n v="9.7841830103138108"/>
     <n v="0.9163752403151868"/>
@@ -1001,7 +1074,7 @@
     <x v="3"/>
     <x v="3"/>
     <x v="0"/>
-    <x v="1"/>
+    <n v="2"/>
     <n v="9.6928388782593551"/>
     <n v="9.188288478528257"/>
     <n v="1.054912337690546"/>
@@ -1010,7 +1083,7 @@
     <x v="4"/>
     <x v="0"/>
     <x v="0"/>
-    <x v="1"/>
+    <n v="2"/>
     <n v="9.6594280168472029"/>
     <n v="9.3817139967814676"/>
     <n v="1.0296016293143246"/>
@@ -1019,7 +1092,7 @@
     <x v="4"/>
     <x v="1"/>
     <x v="0"/>
-    <x v="1"/>
+    <n v="2"/>
     <n v="9.1382309020866224"/>
     <n v="9.7341736652060789"/>
     <n v="0.93877828939403452"/>
@@ -1028,7 +1101,7 @@
     <x v="4"/>
     <x v="2"/>
     <x v="0"/>
-    <x v="1"/>
+    <n v="2"/>
     <n v="8.7707896219732895"/>
     <n v="9.6348965219306155"/>
     <n v="0.91031487489352103"/>
@@ -1037,7 +1110,7 @@
     <x v="4"/>
     <x v="3"/>
     <x v="0"/>
-    <x v="1"/>
+    <n v="2"/>
     <n v="9.6928388782593551"/>
     <n v="9.188288478528257"/>
     <n v="1.054912337690546"/>
@@ -1046,7 +1119,7 @@
     <x v="0"/>
     <x v="0"/>
     <x v="0"/>
-    <x v="2"/>
+    <n v="3"/>
     <n v="9.7099613605188004"/>
     <n v="9.0708816151378944"/>
     <n v="1.0704539836915501"/>
@@ -1055,7 +1128,7 @@
     <x v="0"/>
     <x v="1"/>
     <x v="0"/>
-    <x v="2"/>
+    <n v="3"/>
     <n v="9.7641240202175847"/>
     <n v="9.0756849251237313"/>
     <n v="1.0758553322171955"/>
@@ -1064,7 +1137,7 @@
     <x v="0"/>
     <x v="2"/>
     <x v="0"/>
-    <x v="2"/>
+    <n v="3"/>
     <n v="9.7479108766929521"/>
     <n v="9.0957255072324479"/>
     <n v="1.0717024022923647"/>
@@ -1073,7 +1146,7 @@
     <x v="0"/>
     <x v="3"/>
     <x v="0"/>
-    <x v="2"/>
+    <n v="3"/>
     <n v="9.652611175961848"/>
     <n v="9.0897758955825942"/>
     <n v="1.0619195992117669"/>
@@ -1082,7 +1155,7 @@
     <x v="1"/>
     <x v="0"/>
     <x v="0"/>
-    <x v="1"/>
+    <n v="2"/>
     <n v="9.7192498325707817"/>
     <n v="9.1055233048658941"/>
     <n v="1.0674015657482221"/>
@@ -1091,7 +1164,7 @@
     <x v="1"/>
     <x v="1"/>
     <x v="0"/>
-    <x v="2"/>
+    <n v="3"/>
     <n v="9.7343684796821677"/>
     <n v="9.2425471882742229"/>
     <n v="1.0532127433476246"/>
@@ -1100,7 +1173,7 @@
     <x v="1"/>
     <x v="2"/>
     <x v="0"/>
-    <x v="2"/>
+    <n v="3"/>
     <n v="9.7576719465441908"/>
     <n v="9.1782041635194904"/>
     <n v="1.0631352029984149"/>
@@ -1109,7 +1182,7 @@
     <x v="1"/>
     <x v="3"/>
     <x v="0"/>
-    <x v="2"/>
+    <n v="3"/>
     <n v="9.652611175961848"/>
     <n v="9.0897758955825942"/>
     <n v="1.0619195992117669"/>
@@ -1118,7 +1191,7 @@
     <x v="2"/>
     <x v="0"/>
     <x v="0"/>
-    <x v="2"/>
+    <n v="3"/>
     <n v="9.6476075619331496"/>
     <n v="9.2657394585211286"/>
     <n v="1.0412129118373645"/>
@@ -1127,7 +1200,7 @@
     <x v="2"/>
     <x v="1"/>
     <x v="0"/>
-    <x v="2"/>
+    <n v="3"/>
     <n v="9.6094645925440432"/>
     <n v="9.4409774856698014"/>
     <n v="1.0178463625329033"/>
@@ -1136,7 +1209,7 @@
     <x v="2"/>
     <x v="2"/>
     <x v="0"/>
-    <x v="2"/>
+    <n v="3"/>
     <n v="9.6231261561496613"/>
     <n v="9.4378488809901029"/>
     <n v="1.0196313034353355"/>
@@ -1145,7 +1218,7 @@
     <x v="2"/>
     <x v="3"/>
     <x v="0"/>
-    <x v="2"/>
+    <n v="3"/>
     <n v="9.652611175961848"/>
     <n v="9.0897758955825942"/>
     <n v="1.0619195992117669"/>
@@ -1154,7 +1227,7 @@
     <x v="3"/>
     <x v="0"/>
     <x v="0"/>
-    <x v="2"/>
+    <n v="3"/>
     <n v="9.7205567964501576"/>
     <n v="9.0395906230238126"/>
     <n v="1.0753315279225064"/>
@@ -1163,7 +1236,7 @@
     <x v="3"/>
     <x v="1"/>
     <x v="0"/>
-    <x v="2"/>
+    <n v="3"/>
     <n v="9.4368346463533967"/>
     <n v="9.5616480863226574"/>
     <n v="0.98694645119309521"/>
@@ -1172,7 +1245,7 @@
     <x v="3"/>
     <x v="2"/>
     <x v="0"/>
-    <x v="2"/>
+    <n v="3"/>
     <n v="9.018513939877888"/>
     <n v="9.6618528788088547"/>
     <n v="0.93341453787378725"/>
@@ -1181,7 +1254,7 @@
     <x v="3"/>
     <x v="3"/>
     <x v="0"/>
-    <x v="2"/>
+    <n v="3"/>
     <n v="9.652611175961848"/>
     <n v="9.0897758955825942"/>
     <n v="1.0619195992117669"/>
@@ -1190,7 +1263,7 @@
     <x v="4"/>
     <x v="0"/>
     <x v="0"/>
-    <x v="2"/>
+    <n v="3"/>
     <n v="9.6932762343809227"/>
     <n v="9.1237411303385265"/>
     <n v="1.0624234177522378"/>
@@ -1199,7 +1272,7 @@
     <x v="4"/>
     <x v="1"/>
     <x v="0"/>
-    <x v="2"/>
+    <n v="3"/>
     <n v="9.3249593593677105"/>
     <n v="9.5909217939723863"/>
     <n v="0.97226935634363887"/>
@@ -1208,7 +1281,7 @@
     <x v="4"/>
     <x v="2"/>
     <x v="0"/>
-    <x v="2"/>
+    <n v="3"/>
     <n v="8.923168556064903"/>
     <n v="9.5992185676627813"/>
     <n v="0.92957239104073419"/>
@@ -1217,7 +1290,7 @@
     <x v="4"/>
     <x v="3"/>
     <x v="0"/>
-    <x v="2"/>
+    <n v="3"/>
     <n v="9.652611175961848"/>
     <n v="9.0897758955825942"/>
     <n v="1.0619195992117669"/>
@@ -1226,7 +1299,7 @@
     <x v="0"/>
     <x v="0"/>
     <x v="1"/>
-    <x v="1"/>
+    <n v="2"/>
     <n v="9.7094405342671788"/>
     <n v="9.3459825513836812"/>
     <n v="1.0388892212119192"/>
@@ -1235,7 +1308,7 @@
     <x v="0"/>
     <x v="1"/>
     <x v="1"/>
-    <x v="1"/>
+    <n v="2"/>
     <n v="9.7498297973780002"/>
     <n v="9.3491372883371842"/>
     <n v="1.0428587683208663"/>
@@ -1244,7 +1317,7 @@
     <x v="0"/>
     <x v="2"/>
     <x v="1"/>
-    <x v="1"/>
+    <n v="2"/>
     <n v="9.7748938591456387"/>
     <n v="9.3993598425925029"/>
     <n v="1.0399531481762654"/>
@@ -1253,7 +1326,7 @@
     <x v="0"/>
     <x v="3"/>
     <x v="1"/>
-    <x v="1"/>
+    <n v="2"/>
     <n v="9.6928031367991565"/>
     <n v="9.3323209877780631"/>
     <n v="1.0386272771257219"/>
@@ -1262,7 +1335,7 @@
     <x v="1"/>
     <x v="0"/>
     <x v="1"/>
-    <x v="1"/>
+    <n v="2"/>
     <n v="9.6274107161378559"/>
     <n v="9.0578848546384574"/>
     <n v="1.0628762531914666"/>
@@ -1271,7 +1344,7 @@
     <x v="1"/>
     <x v="1"/>
     <x v="1"/>
-    <x v="1"/>
+    <n v="2"/>
     <n v="9.7706317635284705"/>
     <n v="9.3919682360911416"/>
     <n v="1.0403178032462048"/>
@@ -1280,7 +1353,7 @@
     <x v="1"/>
     <x v="2"/>
     <x v="1"/>
-    <x v="1"/>
+    <n v="2"/>
     <n v="9.6715269614564257"/>
     <n v="9.3965458000882904"/>
     <n v="1.0292640686501577"/>
@@ -1289,7 +1362,7 @@
     <x v="1"/>
     <x v="3"/>
     <x v="1"/>
-    <x v="1"/>
+    <n v="2"/>
     <n v="9.6928031367991565"/>
     <n v="9.3323209877780631"/>
     <n v="1.0386272771257219"/>
@@ -1298,7 +1371,7 @@
     <x v="2"/>
     <x v="0"/>
     <x v="1"/>
-    <x v="1"/>
+    <n v="2"/>
     <n v="9.6941394317298197"/>
     <n v="9.5314037665860809"/>
     <n v="1.0170736304041841"/>
@@ -1307,7 +1380,7 @@
     <x v="2"/>
     <x v="1"/>
     <x v="1"/>
-    <x v="1"/>
+    <n v="2"/>
     <n v="9.5459740954392807"/>
     <n v="9.5511139150615652"/>
     <n v="0.99946186176104768"/>
@@ -1316,7 +1389,7 @@
     <x v="2"/>
     <x v="2"/>
     <x v="1"/>
-    <x v="1"/>
+    <n v="2"/>
     <n v="9.0453053539142036"/>
     <n v="9.753549959702088"/>
     <n v="0.92738596626724845"/>
@@ -1325,7 +1398,7 @@
     <x v="2"/>
     <x v="3"/>
     <x v="1"/>
-    <x v="1"/>
+    <n v="2"/>
     <n v="9.6928031367991565"/>
     <n v="9.3323209877780631"/>
     <n v="1.0386272771257219"/>
@@ -1334,7 +1407,7 @@
     <x v="3"/>
     <x v="0"/>
     <x v="1"/>
-    <x v="1"/>
+    <n v="2"/>
     <n v="9.7084200685368849"/>
     <n v="9.4302288977117357"/>
     <n v="1.0294999383199122"/>
@@ -1343,7 +1416,7 @@
     <x v="3"/>
     <x v="1"/>
     <x v="1"/>
-    <x v="1"/>
+    <n v="2"/>
     <n v="9.4281227003950274"/>
     <n v="9.6226946355856064"/>
     <n v="0.97977989091838846"/>
@@ -1352,7 +1425,7 @@
     <x v="3"/>
     <x v="2"/>
     <x v="1"/>
-    <x v="1"/>
+    <n v="2"/>
     <n v="8.7296962438796157"/>
     <n v="9.5886239181278121"/>
     <n v="0.91042221682880409"/>
@@ -1361,7 +1434,7 @@
     <x v="3"/>
     <x v="3"/>
     <x v="1"/>
-    <x v="1"/>
+    <n v="2"/>
     <n v="9.6928031367991565"/>
     <n v="9.3323209877780631"/>
     <n v="1.0386272771257219"/>
@@ -1370,7 +1443,7 @@
     <x v="4"/>
     <x v="0"/>
     <x v="1"/>
-    <x v="1"/>
+    <n v="2"/>
     <n v="9.4279412150180182"/>
     <n v="9.6435199637586209"/>
     <n v="0.97764522191577652"/>
@@ -1379,7 +1452,7 @@
     <x v="4"/>
     <x v="1"/>
     <x v="1"/>
-    <x v="1"/>
+    <n v="2"/>
     <n v="8.9030899869919438"/>
     <n v="9.5204790866921041"/>
     <n v="0.93515146726563814"/>
@@ -1388,7 +1461,7 @@
     <x v="4"/>
     <x v="2"/>
     <x v="1"/>
-    <x v="1"/>
+    <n v="2"/>
     <n v="8.5536049848239344"/>
     <n v="9.4271530209005405"/>
     <n v="0.90733702591440912"/>
@@ -1397,7 +1470,7 @@
     <x v="4"/>
     <x v="3"/>
     <x v="1"/>
-    <x v="1"/>
+    <n v="2"/>
     <n v="9.6928031367991565"/>
     <n v="9.3323209877780631"/>
     <n v="1.0386272771257219"/>
@@ -1406,7 +1479,7 @@
     <x v="0"/>
     <x v="0"/>
     <x v="1"/>
-    <x v="2"/>
+    <n v="3"/>
     <n v="9.6780129285965621"/>
     <n v="9.0329764901569352"/>
     <n v="1.071409068665518"/>
@@ -1415,7 +1488,7 @@
     <x v="0"/>
     <x v="1"/>
     <x v="1"/>
-    <x v="2"/>
+    <n v="3"/>
     <n v="9.6907560873660117"/>
     <n v="9.0481072926732029"/>
     <n v="1.0710257707944291"/>
@@ -1424,7 +1497,7 @@
     <x v="0"/>
     <x v="2"/>
     <x v="1"/>
-    <x v="2"/>
+    <n v="3"/>
     <n v="9.7404846883769807"/>
     <n v="9.0947451568496831"/>
     <n v="1.0710013882072287"/>
@@ -1433,7 +1506,7 @@
     <x v="0"/>
     <x v="3"/>
     <x v="1"/>
-    <x v="2"/>
+    <n v="3"/>
     <n v="9.6491207892482436"/>
     <n v="9.0312909921140818"/>
     <n v="1.0684099092448285"/>
@@ -1442,7 +1515,7 @@
     <x v="1"/>
     <x v="0"/>
     <x v="1"/>
-    <x v="2"/>
+    <n v="3"/>
     <n v="9.6274107161378559"/>
     <n v="9.0578848546384574"/>
     <n v="1.0628762531914666"/>
@@ -1451,7 +1524,7 @@
     <x v="1"/>
     <x v="1"/>
     <x v="1"/>
-    <x v="2"/>
+    <n v="3"/>
     <n v="9.7706317635284705"/>
     <n v="9.3919682360911416"/>
     <n v="1.0403178032462048"/>
@@ -1460,7 +1533,7 @@
     <x v="1"/>
     <x v="2"/>
     <x v="1"/>
-    <x v="2"/>
+    <n v="3"/>
     <n v="9.672029036225652"/>
     <n v="9.0542825118664183"/>
     <n v="1.0682269990526168"/>
@@ -1469,7 +1542,7 @@
     <x v="1"/>
     <x v="3"/>
     <x v="1"/>
-    <x v="2"/>
+    <n v="3"/>
     <n v="9.6491207892482436"/>
     <n v="9.0312909921140818"/>
     <n v="1.0684099092448285"/>
@@ -1478,7 +1551,7 @@
     <x v="2"/>
     <x v="0"/>
     <x v="1"/>
-    <x v="2"/>
+    <n v="3"/>
     <n v="9.4961441768985466"/>
     <n v="9.1548150837129505"/>
     <n v="1.0372841056934994"/>
@@ -1487,7 +1560,7 @@
     <x v="2"/>
     <x v="1"/>
     <x v="1"/>
-    <x v="2"/>
+    <n v="3"/>
     <n v="9.4534367673610351"/>
     <n v="9.2621331343834896"/>
     <n v="1.020654381685292"/>
@@ -1496,7 +1569,7 @@
     <x v="2"/>
     <x v="2"/>
     <x v="1"/>
-    <x v="2"/>
+    <n v="3"/>
     <n v="9.0453053539142036"/>
     <n v="9.4616479203277528"/>
     <n v="0.95599682318351087"/>
@@ -1505,7 +1578,7 @@
     <x v="2"/>
     <x v="3"/>
     <x v="1"/>
-    <x v="2"/>
+    <n v="3"/>
     <n v="9.6491207892482436"/>
     <n v="9.0312909921140818"/>
     <n v="1.0684099092448285"/>
@@ -1514,7 +1587,7 @@
     <x v="3"/>
     <x v="0"/>
     <x v="1"/>
-    <x v="2"/>
+    <n v="3"/>
     <n v="9.6953969250778336"/>
     <n v="9.188288478528257"/>
     <n v="1.0551907406623788"/>
@@ -1523,7 +1596,7 @@
     <x v="3"/>
     <x v="1"/>
     <x v="1"/>
-    <x v="2"/>
+    <n v="3"/>
     <n v="9.2296962438796157"/>
     <n v="9.4435835104473878"/>
     <n v="0.97735104832491293"/>
@@ -1532,7 +1605,7 @@
     <x v="3"/>
     <x v="2"/>
     <x v="1"/>
-    <x v="2"/>
+    <n v="3"/>
     <n v="8.6855339311358684"/>
     <n v="9.5464304716694102"/>
     <n v="0.90982005859798665"/>
@@ -1541,7 +1614,7 @@
     <x v="3"/>
     <x v="3"/>
     <x v="1"/>
-    <x v="2"/>
+    <n v="3"/>
     <n v="9.6491207892482436"/>
     <n v="9.0312909921140818"/>
     <n v="1.0684099092448285"/>
@@ -1550,7 +1623,7 @@
     <x v="4"/>
     <x v="0"/>
     <x v="1"/>
-    <x v="2"/>
+    <n v="3"/>
     <n v="9.5393733671368039"/>
     <n v="9.2843941061576736"/>
     <n v="1.0274632095604408"/>
@@ -1559,7 +1632,7 @@
     <x v="4"/>
     <x v="1"/>
     <x v="1"/>
-    <x v="2"/>
+    <n v="3"/>
     <n v="9.0435356029532681"/>
     <n v="9.4730295301925622"/>
     <n v="0.95466139677170803"/>
@@ -1568,7 +1641,7 @@
     <x v="4"/>
     <x v="2"/>
     <x v="1"/>
-    <x v="2"/>
+    <n v="3"/>
     <n v="9.0340929308730811"/>
     <n v="9.3050638065379978"/>
     <n v="0.97087920284065921"/>
@@ -1577,7 +1650,7 @@
     <x v="4"/>
     <x v="3"/>
     <x v="1"/>
-    <x v="2"/>
+    <n v="3"/>
     <n v="9.6491207892482436"/>
     <n v="9.0312909921140818"/>
     <n v="1.0684099092448285"/>
@@ -1586,7 +1659,7 @@
     <x v="0"/>
     <x v="0"/>
     <x v="2"/>
-    <x v="1"/>
+    <n v="2"/>
     <n v="9.4771212547196626"/>
     <n v="9.3996702747267911"/>
     <n v="1.0082397549838653"/>
@@ -1595,7 +1668,7 @@
     <x v="0"/>
     <x v="1"/>
     <x v="2"/>
-    <x v="1"/>
+    <n v="2"/>
     <n v="9.4697596263093082"/>
     <n v="9.4542425094393252"/>
     <n v="1.0016412861056283"/>
@@ -1604,7 +1677,7 @@
     <x v="0"/>
     <x v="2"/>
     <x v="2"/>
-    <x v="1"/>
+    <n v="2"/>
     <n v="9.5322289946134582"/>
     <n v="9.5909217939723863"/>
     <n v="0.99388037973619858"/>
@@ -1613,7 +1686,7 @@
     <x v="0"/>
     <x v="3"/>
     <x v="2"/>
-    <x v="1"/>
+    <n v="2"/>
     <n v="9.4373567747804366"/>
     <n v="9.5085166696493904"/>
     <n v="0.99251619391948986"/>
@@ -1622,7 +1695,7 @@
     <x v="1"/>
     <x v="0"/>
     <x v="2"/>
-    <x v="1"/>
+    <n v="2"/>
     <n v="9.4013801308593674"/>
     <n v="9.4228587880360166"/>
     <n v="0.9977205795332601"/>
@@ -1631,7 +1704,7 @@
     <x v="1"/>
     <x v="1"/>
     <x v="2"/>
-    <x v="1"/>
+    <n v="2"/>
     <n v="9.524609011335091"/>
     <n v="9.4818939136727778"/>
     <n v="1.0045049119987219"/>
@@ -1640,7 +1713,7 @@
     <x v="1"/>
     <x v="2"/>
     <x v="2"/>
-    <x v="1"/>
+    <n v="2"/>
     <n v="9.524609011335091"/>
     <n v="9.4818939136727778"/>
     <n v="1.0045049119987219"/>
@@ -1649,7 +1722,7 @@
     <x v="1"/>
     <x v="3"/>
     <x v="2"/>
-    <x v="1"/>
+    <n v="2"/>
     <n v="9.43753063169585"/>
     <n v="9.5085166696493904"/>
     <n v="0.99253447825567542"/>
@@ -1658,7 +1731,7 @@
     <x v="2"/>
     <x v="0"/>
     <x v="2"/>
-    <x v="1"/>
+    <n v="2"/>
     <n v="9.2781512503836439"/>
     <n v="9.4978175972987753"/>
     <n v="0.97687191350383418"/>
@@ -1667,7 +1740,7 @@
     <x v="2"/>
     <x v="1"/>
     <x v="2"/>
-    <x v="1"/>
+    <n v="2"/>
     <n v="9.1152244606891379"/>
     <n v="9.5536049848239344"/>
     <n v="0.95411360163716508"/>
@@ -1676,7 +1749,7 @@
     <x v="2"/>
     <x v="2"/>
     <x v="2"/>
-    <x v="1"/>
+    <n v="2"/>
     <n v="8.8890756251918219"/>
     <n v="9.655876930527878"/>
     <n v="0.92058708796176258"/>
@@ -1685,7 +1758,7 @@
     <x v="2"/>
     <x v="3"/>
     <x v="2"/>
-    <x v="1"/>
+    <n v="2"/>
     <n v="9.43753063169585"/>
     <n v="9.5085166696493904"/>
     <n v="0.99253447825567542"/>
@@ -1694,7 +1767,7 @@
     <x v="3"/>
     <x v="0"/>
     <x v="2"/>
-    <x v="1"/>
+    <n v="2"/>
     <n v="9.524609011335091"/>
     <n v="9.462139643030941"/>
     <n v="1.006602034070609"/>
@@ -1703,7 +1776,7 @@
     <x v="3"/>
     <x v="1"/>
     <x v="2"/>
-    <x v="1"/>
+    <n v="2"/>
     <n v="9.2385606273598313"/>
     <n v="9.6662192299578038"/>
     <n v="0.95575740706639867"/>
@@ -1712,7 +1785,7 @@
     <x v="3"/>
     <x v="2"/>
     <x v="2"/>
-    <x v="1"/>
+    <n v="2"/>
     <n v="8.8890756251918219"/>
     <n v="9.43753063169585"/>
     <n v="0.94188575084863324"/>
@@ -1721,7 +1794,7 @@
     <x v="3"/>
     <x v="3"/>
     <x v="2"/>
-    <x v="1"/>
+    <n v="2"/>
     <n v="9.43753063169585"/>
     <n v="9.5085166696493904"/>
     <n v="0.99253447825567542"/>
@@ -1730,7 +1803,7 @@
     <x v="4"/>
     <x v="0"/>
     <x v="2"/>
-    <x v="1"/>
+    <n v="2"/>
     <n v="9.0395906230238126"/>
     <n v="9.5467108425811169"/>
     <n v="0.94688011107496839"/>
@@ -1739,7 +1812,7 @@
     <x v="4"/>
     <x v="1"/>
     <x v="2"/>
-    <x v="1"/>
+    <n v="2"/>
     <n v="8.6989700043360187"/>
     <n v="9.5322289946134582"/>
     <n v="0.91258508469023314"/>
@@ -1748,7 +1821,7 @@
     <x v="4"/>
     <x v="2"/>
     <x v="2"/>
-    <x v="1"/>
+    <n v="2"/>
     <n v="8.3010299956639813"/>
     <n v="9.4697596263093082"/>
     <n v="0.87658296759737064"/>
@@ -1757,7 +1830,7 @@
     <x v="4"/>
     <x v="3"/>
     <x v="2"/>
-    <x v="1"/>
+    <n v="2"/>
     <n v="9.43753063169585"/>
     <n v="9.5085166696493904"/>
     <n v="0.99253447825567542"/>
@@ -1766,7 +1839,7 @@
     <x v="0"/>
     <x v="0"/>
     <x v="2"/>
-    <x v="2"/>
+    <n v="3"/>
     <n v="9.4911356165197844"/>
     <n v="9.2525749891599531"/>
     <n v="1.0257831606487191"/>
@@ -1775,7 +1848,7 @@
     <x v="0"/>
     <x v="1"/>
     <x v="2"/>
-    <x v="2"/>
+    <n v="3"/>
     <n v="9.5467108425811169"/>
     <n v="9.2898917983084051"/>
     <n v="1.0276449984400762"/>
@@ -1784,7 +1857,7 @@
     <x v="0"/>
     <x v="2"/>
     <x v="2"/>
-    <x v="2"/>
+    <n v="3"/>
     <n v="9.5730640178391191"/>
     <n v="9.4818939136727778"/>
     <n v="1.0096151786759473"/>
@@ -1793,7 +1866,7 @@
     <x v="0"/>
     <x v="3"/>
     <x v="2"/>
-    <x v="2"/>
+    <n v="3"/>
     <n v="9.462139643030941"/>
     <n v="9.2385606273598313"/>
     <n v="1.0242006330519697"/>
@@ -1802,7 +1875,7 @@
     <x v="1"/>
     <x v="0"/>
     <x v="2"/>
-    <x v="2"/>
+    <n v="3"/>
     <n v="9.4373567747804366"/>
     <n v="9.3280443391099439"/>
     <n v="1.0117186874007638"/>
@@ -1811,7 +1884,7 @@
     <x v="1"/>
     <x v="1"/>
     <x v="2"/>
-    <x v="2"/>
+    <n v="3"/>
     <n v="9.4013801308593674"/>
     <n v="9.4228587880360166"/>
     <n v="0.9977205795332601"/>
@@ -1820,7 +1893,7 @@
     <x v="1"/>
     <x v="2"/>
     <x v="2"/>
-    <x v="2"/>
+    <n v="3"/>
     <n v="9.3890756251918219"/>
     <n v="9.2235790156711097"/>
     <n v="1.0179427757098984"/>
@@ -1829,7 +1902,7 @@
     <x v="1"/>
     <x v="3"/>
     <x v="2"/>
-    <x v="2"/>
+    <n v="3"/>
     <n v="9.462139643030941"/>
     <n v="9.2385606273598313"/>
     <n v="1.0242006330519697"/>
@@ -1838,7 +1911,7 @@
     <x v="2"/>
     <x v="0"/>
     <x v="2"/>
-    <x v="2"/>
+    <n v="3"/>
     <n v="9.3010299956639813"/>
     <n v="9.4286662482156345"/>
     <n v="0.98646295783607696"/>
@@ -1847,7 +1920,7 @@
     <x v="2"/>
     <x v="1"/>
     <x v="2"/>
-    <x v="2"/>
+    <n v="3"/>
     <n v="9.2385606273598313"/>
     <n v="9.3217263382430939"/>
     <n v="0.99107829302582406"/>
@@ -1856,7 +1929,7 @@
     <x v="2"/>
     <x v="2"/>
     <x v="2"/>
-    <x v="2"/>
+    <n v="3"/>
     <n v="8.9225490200071285"/>
     <n v="9.4818939136727778"/>
     <n v="0.9410091592715375"/>
@@ -1865,7 +1938,7 @@
     <x v="2"/>
     <x v="3"/>
     <x v="2"/>
-    <x v="2"/>
+    <n v="3"/>
     <n v="9.462139643030941"/>
     <n v="9.2385606273598313"/>
     <n v="1.0242006330519697"/>
@@ -1874,7 +1947,7 @@
     <x v="3"/>
     <x v="0"/>
     <x v="2"/>
-    <x v="2"/>
+    <n v="3"/>
     <n v="9.43753063169585"/>
     <n v="9.2657394585211286"/>
     <n v="1.0185404709406907"/>
@@ -1883,7 +1956,7 @@
     <x v="3"/>
     <x v="1"/>
     <x v="2"/>
-    <x v="2"/>
+    <n v="3"/>
     <n v="8.9771212547196626"/>
     <n v="9.4194245453686278"/>
     <n v="0.95304349129624499"/>
@@ -1892,7 +1965,7 @@
     <x v="3"/>
     <x v="2"/>
     <x v="2"/>
-    <x v="2"/>
+    <n v="3"/>
     <n v="8.4771212547196626"/>
     <n v="9.4313637641589878"/>
     <n v="0.89882242554723291"/>
@@ -1901,7 +1974,7 @@
     <x v="3"/>
     <x v="3"/>
     <x v="2"/>
-    <x v="2"/>
+    <n v="3"/>
     <n v="9.462139643030941"/>
     <n v="9.2385606273598313"/>
     <n v="1.0242006330519697"/>
@@ -1910,7 +1983,7 @@
     <x v="4"/>
     <x v="0"/>
     <x v="2"/>
-    <x v="2"/>
+    <n v="3"/>
     <n v="9.2525749891599531"/>
     <n v="9.3890756251918219"/>
     <n v="0.98546175987062834"/>
@@ -1919,7 +1992,7 @@
     <x v="4"/>
     <x v="1"/>
     <x v="2"/>
-    <x v="2"/>
+    <n v="3"/>
     <n v="8.7385606273598313"/>
     <n v="9.4097719677709346"/>
     <n v="0.92866869221591719"/>
@@ -1928,7 +2001,7 @@
     <x v="4"/>
     <x v="2"/>
     <x v="2"/>
-    <x v="2"/>
+    <n v="3"/>
     <n v="8.4771212547196626"/>
     <n v="9.1461280356782382"/>
     <n v="0.92685355175995354"/>
@@ -1937,7 +2010,7 @@
     <x v="4"/>
     <x v="3"/>
     <x v="2"/>
-    <x v="2"/>
+    <n v="3"/>
     <n v="9.462139643030941"/>
     <n v="9.2385606273598313"/>
     <n v="1.0242006330519697"/>
@@ -1946,7 +2019,7 @@
     <x v="0"/>
     <x v="0"/>
     <x v="0"/>
-    <x v="3"/>
+    <n v="4"/>
     <n v="9.7474111129718892"/>
     <n v="8.9316614300602275"/>
     <n v="1.0913323561690538"/>
@@ -1955,7 +2028,7 @@
     <x v="0"/>
     <x v="1"/>
     <x v="0"/>
-    <x v="3"/>
+    <n v="4"/>
     <n v="9.7648306503268429"/>
     <n v="8.9404067961403957"/>
     <n v="1.092213237382258"/>
@@ -1964,7 +2037,7 @@
     <x v="0"/>
     <x v="2"/>
     <x v="0"/>
-    <x v="3"/>
+    <n v="4"/>
     <n v="9.7460937343654059"/>
     <n v="8.9799974191642082"/>
     <n v="1.0853114181933139"/>
@@ -1973,7 +2046,7 @@
     <x v="0"/>
     <x v="3"/>
     <x v="0"/>
-    <x v="3"/>
+    <n v="4"/>
     <n v="9.6832675093811851"/>
     <n v="9.0025902562518905"/>
     <n v="1.0756090451474891"/>
@@ -1982,7 +2055,7 @@
     <x v="1"/>
     <x v="0"/>
     <x v="0"/>
-    <x v="3"/>
+    <n v="4"/>
     <n v="9.7015602605879092"/>
     <n v="8.9854058054362582"/>
     <n v="1.0797019601183033"/>
@@ -1991,7 +2064,7 @@
     <x v="1"/>
     <x v="1"/>
     <x v="0"/>
-    <x v="3"/>
+    <n v="4"/>
     <n v="9.6787387270694492"/>
     <n v="9.0815806874885094"/>
     <n v="1.0657548570155448"/>
@@ -2000,7 +2073,7 @@
     <x v="1"/>
     <x v="2"/>
     <x v="0"/>
-    <x v="3"/>
+    <n v="4"/>
     <n v="9.6967963750834514"/>
     <n v="9.103412938015925"/>
     <n v="1.0651825245221551"/>
@@ -2009,7 +2082,7 @@
     <x v="1"/>
     <x v="3"/>
     <x v="0"/>
-    <x v="3"/>
+    <n v="4"/>
     <n v="9.6832675093811851"/>
     <n v="9.0025902562518905"/>
     <n v="1.0756090451474891"/>
@@ -2018,7 +2091,7 @@
     <x v="2"/>
     <x v="0"/>
     <x v="0"/>
-    <x v="3"/>
+    <n v="4"/>
     <n v="9.7026219399316531"/>
     <n v="8.9978175972987753"/>
     <n v="1.0783305879466223"/>
@@ -2027,7 +2100,7 @@
     <x v="2"/>
     <x v="1"/>
     <x v="0"/>
-    <x v="3"/>
+    <n v="4"/>
     <n v="9.6069978081840439"/>
     <n v="9.2259699346825528"/>
     <n v="1.0412994922158936"/>
@@ -2036,7 +2109,7 @@
     <x v="2"/>
     <x v="2"/>
     <x v="0"/>
-    <x v="3"/>
+    <n v="4"/>
     <n v="9.7405205573608491"/>
     <n v="9.1704202749061672"/>
     <n v="1.0621673015373896"/>
@@ -2045,7 +2118,7 @@
     <x v="2"/>
     <x v="3"/>
     <x v="0"/>
-    <x v="3"/>
+    <n v="4"/>
     <n v="9.6832675093811851"/>
     <n v="9.0025902562518905"/>
     <n v="1.0756090451474891"/>
@@ -2054,7 +2127,7 @@
     <x v="3"/>
     <x v="0"/>
     <x v="0"/>
-    <x v="3"/>
+    <n v="4"/>
     <n v="9.6857186587020507"/>
     <n v="9.0163093804253602"/>
     <n v="1.0742442666985226"/>
@@ -2063,7 +2136,7 @@
     <x v="3"/>
     <x v="1"/>
     <x v="0"/>
-    <x v="3"/>
+    <n v="4"/>
     <n v="9.2503925864587284"/>
     <n v="9.713475106827488"/>
     <n v="0.9523257623789797"/>
@@ -2072,7 +2145,7 @@
     <x v="3"/>
     <x v="2"/>
     <x v="0"/>
-    <x v="3"/>
+    <n v="4"/>
     <n v="8.9945023078492685"/>
     <n v="9.6621412276488456"/>
     <n v="0.93090155649049255"/>
@@ -2081,7 +2154,7 @@
     <x v="3"/>
     <x v="3"/>
     <x v="0"/>
-    <x v="3"/>
+    <n v="4"/>
     <n v="9.6832675093811851"/>
     <n v="9.0025902562518905"/>
     <n v="1.0756090451474891"/>
@@ -2090,7 +2163,7 @@
     <x v="4"/>
     <x v="0"/>
     <x v="0"/>
-    <x v="3"/>
+    <n v="4"/>
     <n v="9.6848861442984813"/>
     <n v="9.221396612969885"/>
     <n v="1.0502624006733101"/>
@@ -2099,7 +2172,7 @@
     <x v="4"/>
     <x v="1"/>
     <x v="0"/>
-    <x v="3"/>
+    <n v="4"/>
     <n v="9.013674803887378"/>
     <n v="9.7217019084435634"/>
     <n v="0.92717045726929304"/>
@@ -2108,7 +2181,7 @@
     <x v="4"/>
     <x v="2"/>
     <x v="0"/>
-    <x v="3"/>
+    <n v="4"/>
     <n v="8.691907682990216"/>
     <n v="9.6476735741668094"/>
     <n v="0.900933019361703"/>
@@ -2117,7 +2190,7 @@
     <x v="4"/>
     <x v="3"/>
     <x v="0"/>
-    <x v="3"/>
+    <n v="4"/>
     <n v="9.6832675093811851"/>
     <n v="9.0025902562518905"/>
     <n v="1.0756090451474891"/>
@@ -2126,7 +2199,7 @@
     <x v="0"/>
     <x v="0"/>
     <x v="0"/>
-    <x v="4"/>
+    <n v="5"/>
     <n v="9.646670226324348"/>
     <n v="8.6760912590556813"/>
     <n v="1.1118682294006099"/>
@@ -2135,7 +2208,7 @@
     <x v="0"/>
     <x v="1"/>
     <x v="0"/>
-    <x v="4"/>
+    <n v="5"/>
     <n v="9.6206985208248241"/>
     <n v="8.6505149978319906"/>
     <n v="1.1121532675495023"/>
@@ -2144,7 +2217,7 @@
     <x v="0"/>
     <x v="2"/>
     <x v="0"/>
-    <x v="4"/>
+    <n v="5"/>
     <n v="9.6242196040707562"/>
     <n v="8.6760912590556813"/>
     <n v="1.1092805869262226"/>
@@ -2153,7 +2226,7 @@
     <x v="0"/>
     <x v="3"/>
     <x v="0"/>
-    <x v="4"/>
+    <n v="5"/>
     <n v="9.514894735415929"/>
     <n v="8.9304683103500473"/>
     <n v="1.0654418564352952"/>
@@ -2162,7 +2235,7 @@
     <x v="1"/>
     <x v="0"/>
     <x v="0"/>
-    <x v="4"/>
+    <n v="5"/>
     <n v="9.6193742196406227"/>
     <n v="8.6901056208558032"/>
     <n v="1.1069340971592592"/>
@@ -2171,7 +2244,7 @@
     <x v="1"/>
     <x v="1"/>
     <x v="0"/>
-    <x v="4"/>
+    <n v="5"/>
     <n v="9.6433404846774646"/>
     <n v="8.7539279358479156"/>
     <n v="1.1016015388003533"/>
@@ -2180,7 +2253,7 @@
     <x v="1"/>
     <x v="2"/>
     <x v="0"/>
-    <x v="4"/>
+    <n v="5"/>
     <n v="9.6305124169961989"/>
     <n v="8.7512135599922161"/>
     <n v="1.1004773624796291"/>
@@ -2189,7 +2262,7 @@
     <x v="1"/>
     <x v="3"/>
     <x v="0"/>
-    <x v="4"/>
+    <n v="5"/>
     <n v="9.514894735415929"/>
     <n v="8.9304683103500473"/>
     <n v="1.0654418564352952"/>
@@ -2198,7 +2271,7 @@
     <x v="2"/>
     <x v="0"/>
     <x v="0"/>
-    <x v="4"/>
+    <n v="5"/>
     <n v="9.5720067328931009"/>
     <n v="8.6505149978319906"/>
     <n v="1.106524494240176"/>
@@ -2207,7 +2280,7 @@
     <x v="2"/>
     <x v="1"/>
     <x v="0"/>
-    <x v="4"/>
+    <n v="5"/>
     <n v="9.5167118777434752"/>
     <n v="8.8802112417116064"/>
     <n v="1.0716762944829663"/>
@@ -2216,7 +2289,7 @@
     <x v="2"/>
     <x v="2"/>
     <x v="0"/>
-    <x v="4"/>
+    <n v="5"/>
     <n v="9.6166503857817354"/>
     <n v="8.8419735653757563"/>
     <n v="1.0876135644014513"/>
@@ -2225,7 +2298,7 @@
     <x v="2"/>
     <x v="3"/>
     <x v="0"/>
-    <x v="4"/>
+    <n v="5"/>
     <n v="9.514894735415929"/>
     <n v="8.9304683103500473"/>
     <n v="1.0654418564352952"/>
@@ -2234,7 +2307,7 @@
     <x v="3"/>
     <x v="0"/>
     <x v="0"/>
-    <x v="4"/>
+    <n v="5"/>
     <n v="9.5962279692559882"/>
     <n v="8.6808639180087965"/>
     <n v="1.1054461929011734"/>
@@ -2243,7 +2316,7 @@
     <x v="3"/>
     <x v="1"/>
     <x v="0"/>
-    <x v="4"/>
+    <n v="5"/>
     <n v="9.3277612981267097"/>
     <n v="9.3162286460923625"/>
     <n v="1.0012379099389306"/>
@@ -2252,7 +2325,7 @@
     <x v="3"/>
     <x v="2"/>
     <x v="0"/>
-    <x v="4"/>
+    <n v="5"/>
     <n v="9.3090240483560471"/>
     <n v="9.3459825513836812"/>
     <n v="0.99604551979158551"/>
@@ -2261,7 +2334,7 @@
     <x v="3"/>
     <x v="3"/>
     <x v="0"/>
-    <x v="4"/>
+    <n v="5"/>
     <n v="9.514894735415929"/>
     <n v="8.9304683103500473"/>
     <n v="1.0654418564352952"/>
@@ -2270,7 +2343,7 @@
     <x v="4"/>
     <x v="0"/>
     <x v="0"/>
-    <x v="4"/>
+    <n v="5"/>
     <n v="9.5783351382770636"/>
     <n v="8.9259348003648835"/>
     <n v="1.0730904216200987"/>
@@ -2279,7 +2352,7 @@
     <x v="4"/>
     <x v="1"/>
     <x v="0"/>
-    <x v="4"/>
+    <n v="5"/>
     <n v="9.2659947757062753"/>
     <n v="9.4534367673610351"/>
     <n v="0.98017207960792385"/>
@@ -2288,7 +2361,7 @@
     <x v="4"/>
     <x v="2"/>
     <x v="0"/>
-    <x v="4"/>
+    <n v="5"/>
     <n v="8.9763962215220463"/>
     <n v="9.4947249088333461"/>
     <n v="0.9454087725249336"/>
@@ -2297,7 +2370,7 @@
     <x v="4"/>
     <x v="3"/>
     <x v="0"/>
-    <x v="4"/>
+    <n v="5"/>
     <n v="9.514894735415929"/>
     <n v="8.9304683103500473"/>
     <n v="1.0654418564352952"/>
@@ -2306,7 +2379,7 @@
     <x v="0"/>
     <x v="0"/>
     <x v="1"/>
-    <x v="3"/>
+    <n v="4"/>
     <n v="9.5936757411117313"/>
     <n v="9.2825695759848941"/>
     <n v="1.033515091115687"/>
@@ -2315,7 +2388,7 @@
     <x v="0"/>
     <x v="1"/>
     <x v="1"/>
-    <x v="3"/>
+    <n v="4"/>
     <n v="9.6991870430756784"/>
     <n v="9.2579369218558405"/>
     <n v="1.0476618197925014"/>
@@ -2324,7 +2397,7 @@
     <x v="0"/>
     <x v="2"/>
     <x v="1"/>
-    <x v="3"/>
+    <n v="4"/>
     <n v="9.6249170207983958"/>
     <n v="9.2631696386949223"/>
     <n v="1.0390522246934084"/>
@@ -2333,7 +2406,7 @@
     <x v="0"/>
     <x v="3"/>
     <x v="1"/>
-    <x v="3"/>
+    <n v="4"/>
     <n v="9.5204988462117441"/>
     <n v="9.2988475929627565"/>
     <n v="1.023836421775181"/>
@@ -2342,7 +2415,7 @@
     <x v="1"/>
     <x v="0"/>
     <x v="1"/>
-    <x v="3"/>
+    <n v="4"/>
     <n v="9.5286428222091075"/>
     <n v="9.2645225853828848"/>
     <n v="1.0285087800684882"/>
@@ -2351,7 +2424,7 @@
     <x v="1"/>
     <x v="1"/>
     <x v="1"/>
-    <x v="3"/>
+    <n v="4"/>
     <n v="9.5711947330594178"/>
     <n v="9.3167847212770454"/>
     <n v="1.0273066319973421"/>
@@ -2360,7 +2433,7 @@
     <x v="1"/>
     <x v="2"/>
     <x v="1"/>
-    <x v="3"/>
+    <n v="4"/>
     <n v="9.5035323281891664"/>
     <n v="9.3063919283598686"/>
     <n v="1.0211833330625741"/>
@@ -2369,7 +2442,7 @@
     <x v="1"/>
     <x v="3"/>
     <x v="1"/>
-    <x v="3"/>
+    <n v="4"/>
     <n v="9.5204988462117441"/>
     <n v="9.2988475929627565"/>
     <n v="1.023836421775181"/>
@@ -2378,7 +2451,7 @@
     <x v="2"/>
     <x v="0"/>
     <x v="1"/>
-    <x v="3"/>
+    <n v="4"/>
     <n v="9.4501835643282348"/>
     <n v="9.3502653284892965"/>
     <n v="1.0106861390911013"/>
@@ -2387,7 +2460,7 @@
     <x v="2"/>
     <x v="1"/>
     <x v="1"/>
-    <x v="3"/>
+    <n v="4"/>
     <n v="9.0633902885060049"/>
     <n v="9.429298672497346"/>
     <n v="0.96119452817221762"/>
@@ -2396,7 +2469,7 @@
     <x v="2"/>
     <x v="2"/>
     <x v="1"/>
-    <x v="3"/>
+    <n v="4"/>
     <n v="9.0481072926732029"/>
     <n v="9.631320451877631"/>
     <n v="0.93944618890852805"/>
@@ -2405,7 +2478,7 @@
     <x v="2"/>
     <x v="3"/>
     <x v="1"/>
-    <x v="3"/>
+    <n v="4"/>
     <n v="9.5204988462117441"/>
     <n v="9.2988475929627565"/>
     <n v="1.023836421775181"/>
@@ -2414,7 +2487,7 @@
     <x v="3"/>
     <x v="0"/>
     <x v="1"/>
-    <x v="3"/>
+    <n v="4"/>
     <n v="9.6101194399672032"/>
     <n v="9.3141944650251567"/>
     <n v="1.0317713975216265"/>
@@ -2423,7 +2496,7 @@
     <x v="3"/>
     <x v="1"/>
     <x v="1"/>
-    <x v="3"/>
+    <n v="4"/>
     <n v="9.2769415133219368"/>
     <n v="9.5057429299997018"/>
     <n v="0.97593019100530498"/>
@@ -2432,7 +2505,7 @@
     <x v="3"/>
     <x v="2"/>
     <x v="1"/>
-    <x v="3"/>
+    <n v="4"/>
     <n v="8.9515449934959719"/>
     <n v="9.2075701760979367"/>
     <n v="0.97219405579263629"/>
@@ -2441,7 +2514,7 @@
     <x v="3"/>
     <x v="3"/>
     <x v="1"/>
-    <x v="3"/>
+    <n v="4"/>
     <n v="9.5204988462117441"/>
     <n v="9.2988475929627565"/>
     <n v="1.023836421775181"/>
@@ -2450,7 +2523,7 @@
     <x v="4"/>
     <x v="0"/>
     <x v="1"/>
-    <x v="3"/>
+    <n v="4"/>
     <n v="9.2633634336573181"/>
     <n v="9.4057875029352971"/>
     <n v="0.98485782618057949"/>
@@ -2459,7 +2532,7 @@
     <x v="4"/>
     <x v="1"/>
     <x v="1"/>
-    <x v="3"/>
+    <n v="4"/>
     <n v="9.0163093804253602"/>
     <n v="9.3955996232494385"/>
     <n v="0.9596310764578001"/>
@@ -2468,7 +2541,7 @@
     <x v="4"/>
     <x v="2"/>
     <x v="1"/>
-    <x v="3"/>
+    <n v="4"/>
     <n v="9.0167118777434752"/>
     <n v="9.288745899918613"/>
     <n v="0.97071358985312306"/>
@@ -2477,7 +2550,7 @@
     <x v="4"/>
     <x v="3"/>
     <x v="1"/>
-    <x v="3"/>
+    <n v="4"/>
     <n v="9.5204988462117441"/>
     <n v="9.2988475929627565"/>
     <n v="1.023836421775181"/>
@@ -2486,7 +2559,7 @@
     <x v="0"/>
     <x v="0"/>
     <x v="1"/>
-    <x v="4"/>
+    <n v="5"/>
     <n v="9.5606321526147902"/>
     <n v="9.1487708339090794"/>
     <n v="1.0450182135046147"/>
@@ -2495,7 +2568,7 @@
     <x v="0"/>
     <x v="1"/>
     <x v="1"/>
-    <x v="4"/>
+    <n v="5"/>
     <n v="9.5511139150615652"/>
     <n v="9.0641996343589035"/>
     <n v="1.0537183976902889"/>
@@ -2504,7 +2577,7 @@
     <x v="0"/>
     <x v="2"/>
     <x v="1"/>
-    <x v="4"/>
+    <n v="5"/>
     <n v="9.6721863109532364"/>
     <n v="9.2083202536691395"/>
     <n v="1.0503746660091742"/>
@@ -2513,7 +2586,7 @@
     <x v="0"/>
     <x v="3"/>
     <x v="1"/>
-    <x v="4"/>
+    <n v="5"/>
     <n v="9.530839307622669"/>
     <n v="9.0897758955825942"/>
     <n v="1.0485230237914249"/>
@@ -2522,7 +2595,7 @@
     <x v="1"/>
     <x v="0"/>
     <x v="1"/>
-    <x v="4"/>
+    <n v="5"/>
     <n v="9.4956351945975506"/>
     <n v="9.1636794671931661"/>
     <n v="1.0362251570008332"/>
@@ -2531,7 +2604,7 @@
     <x v="1"/>
     <x v="1"/>
     <x v="1"/>
-    <x v="4"/>
+    <n v="5"/>
     <n v="9.4100350171561633"/>
     <n v="9.1782041635194904"/>
     <n v="1.0252588468840265"/>
@@ -2540,7 +2613,7 @@
     <x v="1"/>
     <x v="2"/>
     <x v="1"/>
-    <x v="4"/>
+    <n v="5"/>
     <n v="9.3973485634459983"/>
     <n v="9.2491552768948004"/>
     <n v="1.0160223590278994"/>
@@ -2549,7 +2622,7 @@
     <x v="1"/>
     <x v="3"/>
     <x v="1"/>
-    <x v="4"/>
+    <n v="5"/>
     <n v="9.530839307622669"/>
     <n v="9.0897758955825942"/>
     <n v="1.0485230237914249"/>
@@ -2558,7 +2631,7 @@
     <x v="2"/>
     <x v="0"/>
     <x v="1"/>
-    <x v="4"/>
+    <n v="5"/>
     <n v="9.4366603009077004"/>
     <n v="9.1735673914550091"/>
     <n v="1.0286794545923059"/>
@@ -2567,7 +2640,7 @@
     <x v="2"/>
     <x v="1"/>
     <x v="1"/>
-    <x v="4"/>
+    <n v="5"/>
     <n v="8.8512152682227629"/>
     <n v="9.2618732334057832"/>
     <n v="0.95566145693920146"/>
@@ -2576,7 +2649,7 @@
     <x v="2"/>
     <x v="2"/>
     <x v="1"/>
-    <x v="4"/>
+    <n v="5"/>
     <n v="9.0140822097122353"/>
     <n v="9.3593338676581048"/>
     <n v="0.96311151382910776"/>
@@ -2585,7 +2658,7 @@
     <x v="2"/>
     <x v="3"/>
     <x v="1"/>
-    <x v="4"/>
+    <n v="5"/>
     <n v="9.530839307622669"/>
     <n v="9.0897758955825942"/>
     <n v="1.0485230237914249"/>
@@ -2594,7 +2667,7 @@
     <x v="3"/>
     <x v="0"/>
     <x v="1"/>
-    <x v="4"/>
+    <n v="5"/>
     <n v="9.4582269742749627"/>
     <n v="9.0602869656029252"/>
     <n v="1.0439213471033317"/>
@@ -2603,7 +2676,7 @@
     <x v="3"/>
     <x v="1"/>
     <x v="1"/>
-    <x v="4"/>
+    <n v="5"/>
     <n v="9.1975757957522717"/>
     <n v="9.1657136482603718"/>
     <n v="1.0034762320441843"/>
@@ -2612,7 +2685,7 @@
     <x v="3"/>
     <x v="2"/>
     <x v="1"/>
-    <x v="4"/>
+    <n v="5"/>
     <n v="8.6483325951307659"/>
     <n v="8.8512152682227629"/>
     <n v="0.97707855170799229"/>
@@ -2621,7 +2694,7 @@
     <x v="3"/>
     <x v="3"/>
     <x v="1"/>
-    <x v="4"/>
+    <n v="5"/>
     <n v="9.530839307622669"/>
     <n v="9.0897758955825942"/>
     <n v="1.0485230237914249"/>
@@ -2630,7 +2703,7 @@
     <x v="4"/>
     <x v="0"/>
     <x v="1"/>
-    <x v="4"/>
+    <n v="5"/>
     <n v="9.153212513775344"/>
     <n v="9.1721961368425546"/>
     <n v="0.99793030777100833"/>
@@ -2639,7 +2712,7 @@
     <x v="4"/>
     <x v="1"/>
     <x v="1"/>
-    <x v="4"/>
+    <n v="5"/>
     <n v="8.8919517896363676"/>
     <n v="9.0503575432865411"/>
     <n v="0.98249729329559166"/>
@@ -2648,7 +2721,7 @@
     <x v="4"/>
     <x v="2"/>
     <x v="1"/>
-    <x v="4"/>
+    <n v="5"/>
     <n v="8.5806840011174863"/>
     <n v="8.8767915294464537"/>
     <n v="0.96664250508230287"/>
@@ -2657,7 +2730,7 @@
     <x v="4"/>
     <x v="3"/>
     <x v="1"/>
-    <x v="4"/>
+    <n v="5"/>
     <n v="9.530839307622669"/>
     <n v="9.0897758955825942"/>
     <n v="1.0485230237914249"/>
@@ -2666,7 +2739,7 @@
     <x v="0"/>
     <x v="0"/>
     <x v="2"/>
-    <x v="3"/>
+    <n v="4"/>
     <n v="9.9213981975877914"/>
     <n v="9.6812412373755876"/>
     <n v="1.0248064224745324"/>
@@ -2675,7 +2748,7 @@
     <x v="0"/>
     <x v="1"/>
     <x v="2"/>
-    <x v="3"/>
+    <n v="4"/>
     <n v="9.9949917291506996"/>
     <n v="9.7623927246606108"/>
     <n v="1.0238260241162522"/>
@@ -2684,7 +2757,7 @@
     <x v="0"/>
     <x v="2"/>
     <x v="2"/>
-    <x v="3"/>
+    <n v="4"/>
     <n v="10.050804808616556"/>
     <n v="9.6690289377098786"/>
     <n v="1.0394844066933884"/>
@@ -2693,7 +2766,7 @@
     <x v="0"/>
     <x v="3"/>
     <x v="2"/>
-    <x v="3"/>
+    <n v="4"/>
     <n v="9.9081206499958903"/>
     <n v="9.557305492116086"/>
     <n v="1.0367064920305409"/>
@@ -2702,7 +2775,7 @@
     <x v="1"/>
     <x v="0"/>
     <x v="2"/>
-    <x v="3"/>
+    <n v="4"/>
     <n v="9.8117280240349665"/>
     <n v="9.7442753582502224"/>
     <n v="1.0069222865020573"/>
@@ -2711,7 +2784,7 @@
     <x v="1"/>
     <x v="1"/>
     <x v="2"/>
-    <x v="3"/>
+    <n v="4"/>
     <n v="9.8883505919942056"/>
     <n v="9.6725888082713531"/>
     <n v="1.0223065187613833"/>
@@ -2720,7 +2793,7 @@
     <x v="1"/>
     <x v="2"/>
     <x v="2"/>
-    <x v="3"/>
+    <n v="4"/>
     <n v="9.8682380910138487"/>
     <n v="9.6929817853003488"/>
     <n v="1.0180807422932827"/>
@@ -2729,7 +2802,7 @@
     <x v="1"/>
     <x v="3"/>
     <x v="2"/>
-    <x v="3"/>
+    <n v="4"/>
     <n v="9.9081206499958903"/>
     <n v="9.557305492116086"/>
     <n v="1.0367064920305409"/>
@@ -2738,7 +2811,7 @@
     <x v="2"/>
     <x v="0"/>
     <x v="2"/>
-    <x v="3"/>
+    <n v="4"/>
     <n v="9.6972258404131075"/>
     <n v="9.6708161678890274"/>
     <n v="1.0027308628419358"/>
@@ -2747,7 +2820,7 @@
     <x v="2"/>
     <x v="1"/>
     <x v="2"/>
-    <x v="3"/>
+    <n v="4"/>
     <n v="9.3222192947339195"/>
     <n v="9.678967423500227"/>
     <n v="0.96314192277369026"/>
@@ -2756,7 +2829,7 @@
     <x v="2"/>
     <x v="2"/>
     <x v="2"/>
-    <x v="3"/>
+    <n v="4"/>
     <n v="9.2428607132407912"/>
     <n v="10.128791293790691"/>
     <n v="0.91253343515005525"/>
@@ -2765,7 +2838,7 @@
     <x v="2"/>
     <x v="3"/>
     <x v="2"/>
-    <x v="3"/>
+    <n v="4"/>
     <n v="9.9081206499958903"/>
     <n v="9.557305492116086"/>
     <n v="1.0367064920305409"/>
@@ -2774,7 +2847,7 @@
     <x v="3"/>
     <x v="0"/>
     <x v="2"/>
-    <x v="3"/>
+    <n v="4"/>
     <n v="9.8710875216118374"/>
     <n v="9.7742561281705171"/>
     <n v="1.009906778804603"/>
@@ -2783,7 +2856,7 @@
     <x v="3"/>
     <x v="1"/>
     <x v="2"/>
-    <x v="3"/>
+    <n v="4"/>
     <n v="9.4262399968184276"/>
     <n v="9.9057875029352971"/>
     <n v="0.95158915876453343"/>
@@ -2792,7 +2865,7 @@
     <x v="3"/>
     <x v="2"/>
     <x v="2"/>
-    <x v="3"/>
+    <n v="4"/>
     <n v="9.2156818820794939"/>
     <n v="9.5902063164191631"/>
     <n v="0.96094719738214029"/>
@@ -2801,7 +2874,7 @@
     <x v="3"/>
     <x v="3"/>
     <x v="2"/>
-    <x v="3"/>
+    <n v="4"/>
     <n v="9.9081206499958903"/>
     <n v="9.557305492116086"/>
     <n v="1.0367064920305409"/>
@@ -2810,7 +2883,7 @@
     <x v="4"/>
     <x v="0"/>
     <x v="2"/>
-    <x v="3"/>
+    <n v="4"/>
     <n v="9.5809833081820379"/>
     <n v="9.7988475929627565"/>
     <n v="0.97776633601922924"/>
@@ -2819,7 +2892,7 @@
     <x v="4"/>
     <x v="1"/>
     <x v="2"/>
-    <x v="3"/>
+    <n v="4"/>
     <n v="8.9978175972987753"/>
     <n v="9.7274224300042551"/>
     <n v="0.92499505002938787"/>
@@ -2828,7 +2901,7 @@
     <x v="4"/>
     <x v="2"/>
     <x v="2"/>
-    <x v="3"/>
+    <n v="4"/>
     <n v="8.7657394585211286"/>
     <n v="9.7801326989313573"/>
     <n v="0.89628021708528882"/>
@@ -2837,7 +2910,7 @@
     <x v="4"/>
     <x v="3"/>
     <x v="2"/>
-    <x v="3"/>
+    <n v="4"/>
     <n v="9.9081206499958903"/>
     <n v="9.557305492116086"/>
     <n v="1.0367064920305409"/>
@@ -2846,7 +2919,7 @@
     <x v="0"/>
     <x v="0"/>
     <x v="2"/>
-    <x v="4"/>
+    <n v="5"/>
     <n v="9.808342760447756"/>
     <n v="9.6493173915622172"/>
     <n v="1.0164804786113262"/>
@@ -2855,7 +2928,7 @@
     <x v="0"/>
     <x v="1"/>
     <x v="2"/>
-    <x v="4"/>
+    <n v="5"/>
     <n v="9.810380244997102"/>
     <n v="9.7075701760979367"/>
     <n v="1.0105907108611283"/>
@@ -2864,7 +2937,7 @@
     <x v="0"/>
     <x v="2"/>
     <x v="2"/>
-    <x v="4"/>
+    <n v="5"/>
     <n v="9.8846886630380695"/>
     <n v="9.7960883786979345"/>
     <n v="1.0090444553902556"/>
@@ -2873,7 +2946,7 @@
     <x v="0"/>
     <x v="3"/>
     <x v="2"/>
-    <x v="4"/>
+    <n v="5"/>
     <n v="9.6812412373755876"/>
     <n v="9.5112141855927437"/>
     <n v="1.0178764822729358"/>
@@ -2882,7 +2955,7 @@
     <x v="1"/>
     <x v="0"/>
     <x v="2"/>
-    <x v="4"/>
+    <n v="5"/>
     <n v="9.8375223679779467"/>
     <n v="9.6803913449366412"/>
     <n v="1.0162318874766869"/>
@@ -2891,7 +2964,7 @@
     <x v="1"/>
     <x v="1"/>
     <x v="2"/>
-    <x v="4"/>
+    <n v="5"/>
     <n v="9.7467987245002625"/>
     <n v="9.5730640178391191"/>
     <n v="1.0181482863101505"/>
@@ -2900,7 +2973,7 @@
     <x v="1"/>
     <x v="2"/>
     <x v="2"/>
-    <x v="4"/>
+    <n v="5"/>
     <n v="9.7711636913869881"/>
     <n v="9.641763682430847"/>
     <n v="1.0134207820496506"/>
@@ -2909,7 +2982,7 @@
     <x v="1"/>
     <x v="3"/>
     <x v="2"/>
-    <x v="4"/>
+    <n v="5"/>
     <n v="9.6812412373755876"/>
     <n v="9.5112141855927437"/>
     <n v="1.0178764822729358"/>
@@ -2918,7 +2991,7 @@
     <x v="2"/>
     <x v="0"/>
     <x v="2"/>
-    <x v="4"/>
+    <n v="5"/>
     <n v="9.704119982655925"/>
     <n v="9.5835108978951276"/>
     <n v="1.0125850626190958"/>
@@ -2927,7 +3000,7 @@
     <x v="2"/>
     <x v="1"/>
     <x v="2"/>
-    <x v="4"/>
+    <n v="5"/>
     <n v="8.8580016718173997"/>
     <n v="9.5021606868913224"/>
     <n v="0.93220920627425607"/>
@@ -2936,7 +3009,7 @@
     <x v="2"/>
     <x v="2"/>
     <x v="2"/>
-    <x v="4"/>
+    <n v="5"/>
     <n v="9.1760912590556813"/>
     <n v="9.8569551770644779"/>
     <n v="0.93092553371927111"/>
@@ -2945,7 +3018,7 @@
     <x v="2"/>
     <x v="3"/>
     <x v="2"/>
-    <x v="4"/>
+    <n v="5"/>
     <n v="9.6812412373755876"/>
     <n v="9.5112141855927437"/>
     <n v="1.0178764822729358"/>
@@ -2954,7 +3027,7 @@
     <x v="3"/>
     <x v="0"/>
     <x v="2"/>
-    <x v="4"/>
+    <n v="5"/>
     <n v="9.8025447309407898"/>
     <n v="9.3890756251918219"/>
     <n v="1.0440372537462144"/>
@@ -2963,7 +3036,7 @@
     <x v="3"/>
     <x v="1"/>
     <x v="2"/>
-    <x v="4"/>
+    <n v="5"/>
     <n v="9.4712520530840401"/>
     <n v="9.6474534553025961"/>
     <n v="0.98173596762763238"/>
@@ -2972,7 +3045,7 @@
     <x v="3"/>
     <x v="2"/>
     <x v="2"/>
-    <x v="4"/>
+    <n v="5"/>
     <n v="8.9119543704721593"/>
     <n v="9.2470772970092217"/>
     <n v="0.96375904344982055"/>
@@ -2981,7 +3054,7 @@
     <x v="3"/>
     <x v="3"/>
     <x v="2"/>
-    <x v="4"/>
+    <n v="5"/>
     <n v="9.6812412373755876"/>
     <n v="9.5112141855927437"/>
     <n v="1.0178764822729358"/>
@@ -2990,7 +3063,7 @@
     <x v="4"/>
     <x v="0"/>
     <x v="2"/>
-    <x v="4"/>
+    <n v="5"/>
     <n v="9.430268818153241"/>
     <n v="9.5789800906456044"/>
     <n v="0.98447524986114254"/>
@@ -2999,7 +3072,7 @@
     <x v="4"/>
     <x v="1"/>
     <x v="2"/>
-    <x v="4"/>
+    <n v="5"/>
     <n v="9.0167118777434752"/>
     <n v="9.3688612966640186"/>
     <n v="0.96241278339279779"/>
@@ -3008,7 +3081,7 @@
     <x v="4"/>
     <x v="2"/>
     <x v="2"/>
-    <x v="4"/>
+    <n v="5"/>
     <n v="8.3634993639681312"/>
     <n v="9.266589350960075"/>
     <n v="0.90254343288683903"/>
@@ -3017,7 +3090,7 @@
     <x v="4"/>
     <x v="3"/>
     <x v="2"/>
-    <x v="4"/>
+    <n v="5"/>
     <n v="9.6812412373755876"/>
     <n v="9.5112141855927437"/>
     <n v="1.0178764822729358"/>
@@ -3026,7 +3099,7 @@
     <x v="0"/>
     <x v="0"/>
     <x v="0"/>
-    <x v="5"/>
+    <n v="6"/>
     <n v="9.0815806874885094"/>
     <n v="9.3798339223448153"/>
     <n v="0.96820271687904824"/>
@@ -3035,7 +3108,7 @@
     <x v="0"/>
     <x v="1"/>
     <x v="0"/>
-    <x v="5"/>
+    <n v="6"/>
     <n v="9.0897758955825942"/>
     <n v="9.4029542275370979"/>
     <n v="0.96669362368718725"/>
@@ -3044,7 +3117,7 @@
     <x v="0"/>
     <x v="2"/>
     <x v="0"/>
-    <x v="5"/>
+    <n v="6"/>
     <n v="9.0809833081820379"/>
     <n v="9.4057875029352971"/>
     <n v="0.96546762356135551"/>
@@ -3053,7 +3126,7 @@
     <x v="0"/>
     <x v="3"/>
     <x v="0"/>
-    <x v="5"/>
+    <n v="6"/>
     <n v="9.0736835538968936"/>
     <n v="9.4084850188786504"/>
     <n v="0.96441494413713169"/>
@@ -3062,7 +3135,7 @@
     <x v="1"/>
     <x v="0"/>
     <x v="0"/>
-    <x v="5"/>
+    <n v="6"/>
     <n v="9.096562299177231"/>
     <n v="9.4285455773367559"/>
     <n v="0.96478955577650194"/>
@@ -3071,7 +3144,7 @@
     <x v="1"/>
     <x v="1"/>
     <x v="0"/>
-    <x v="5"/>
+    <n v="6"/>
     <n v="9.2466593041160507"/>
     <n v="9.3480907935842623"/>
     <n v="0.98914949675736719"/>
@@ -3080,7 +3153,7 @@
     <x v="1"/>
     <x v="2"/>
     <x v="0"/>
-    <x v="5"/>
+    <n v="6"/>
     <n v="9.2466593041160507"/>
     <n v="9.3127076760772045"/>
     <n v="0.99290771553682278"/>
@@ -3089,7 +3162,7 @@
     <x v="1"/>
     <x v="3"/>
     <x v="0"/>
-    <x v="5"/>
+    <n v="6"/>
     <n v="9.0736835538968936"/>
     <n v="9.4084850188786504"/>
     <n v="0.96441494413713169"/>
@@ -3098,7 +3171,7 @@
     <x v="2"/>
     <x v="0"/>
     <x v="0"/>
-    <x v="5"/>
+    <n v="6"/>
     <n v="9.0374082203225878"/>
     <n v="9.424279286061882"/>
     <n v="0.95894953300975916"/>
@@ -3107,7 +3180,7 @@
     <x v="2"/>
     <x v="1"/>
     <x v="0"/>
-    <x v="5"/>
+    <n v="6"/>
     <n v="8.8256390069990722"/>
     <n v="9.4667436439243531"/>
     <n v="0.9322782298708665"/>
@@ -3116,7 +3189,7 @@
     <x v="2"/>
     <x v="2"/>
     <x v="0"/>
-    <x v="5"/>
+    <n v="6"/>
     <n v="9.035941003653063"/>
     <n v="9.3970696778838878"/>
     <n v="0.96157007592688759"/>
@@ -3125,7 +3198,7 @@
     <x v="2"/>
     <x v="3"/>
     <x v="0"/>
-    <x v="5"/>
+    <n v="6"/>
     <n v="9.0736835538968936"/>
     <n v="9.4084850188786504"/>
     <n v="0.96441494413713169"/>
@@ -3134,7 +3207,7 @@
     <x v="3"/>
     <x v="0"/>
     <x v="0"/>
-    <x v="5"/>
+    <n v="6"/>
     <n v="9.0105946495349691"/>
     <n v="9.479663822986085"/>
     <n v="0.95051837467972999"/>
@@ -3143,7 +3216,7 @@
     <x v="3"/>
     <x v="1"/>
     <x v="0"/>
-    <x v="5"/>
+    <n v="6"/>
     <n v="8.484241474276967"/>
     <n v="9.5070291387121681"/>
     <n v="0.89241774170329835"/>
@@ -3152,7 +3225,7 @@
     <x v="3"/>
     <x v="2"/>
     <x v="0"/>
-    <x v="5"/>
+    <n v="6"/>
     <n v="7.9515449934959719"/>
     <n v="9.5230133348512709"/>
     <n v="0.83498202868159255"/>
@@ -3161,7 +3234,7 @@
     <x v="3"/>
     <x v="3"/>
     <x v="0"/>
-    <x v="5"/>
+    <n v="6"/>
     <n v="9.0736835538968936"/>
     <n v="9.4084850188786504"/>
     <n v="0.96441494413713169"/>
@@ -3170,7 +3243,7 @@
     <x v="4"/>
     <x v="0"/>
     <x v="0"/>
-    <x v="5"/>
+    <n v="6"/>
     <n v="8.9117371145851507"/>
     <n v="9.5204988462117441"/>
     <n v="0.93605779051495575"/>
@@ -3179,7 +3252,7 @@
     <x v="4"/>
     <x v="1"/>
     <x v="0"/>
-    <x v="5"/>
+    <n v="6"/>
     <n v="8.4460473013452404"/>
     <n v="9.5464304716694102"/>
     <n v="0.88473354793818104"/>
@@ -3188,7 +3261,7 @@
     <x v="4"/>
     <x v="2"/>
     <x v="0"/>
-    <x v="5"/>
+    <n v="6"/>
     <n v="7.6020599913279625"/>
     <n v="9.5101391970559632"/>
     <n v="0.79936369319192702"/>
@@ -3197,7 +3270,7 @@
     <x v="4"/>
     <x v="3"/>
     <x v="0"/>
-    <x v="5"/>
+    <n v="6"/>
     <n v="9.0736835538968936"/>
     <n v="9.4084850188786504"/>
     <n v="0.96441494413713169"/>
@@ -3206,7 +3279,7 @@
     <x v="0"/>
     <x v="0"/>
     <x v="0"/>
-    <x v="6"/>
+    <n v="7"/>
     <n v="9.6799177411699446"/>
     <n v="9.0542825118664183"/>
     <n v="1.0690982668680349"/>
@@ -3215,7 +3288,7 @@
     <x v="0"/>
     <x v="1"/>
     <x v="0"/>
-    <x v="6"/>
+    <n v="7"/>
     <n v="9.6273223686773122"/>
     <n v="9.0064186123525865"/>
     <n v="1.0689401395881306"/>
@@ -3224,7 +3297,7 @@
     <x v="0"/>
     <x v="2"/>
     <x v="0"/>
-    <x v="6"/>
+    <n v="7"/>
     <n v="9.7225217307250915"/>
     <n v="9.1221385604009217"/>
     <n v="1.0658160546837585"/>
@@ -3233,7 +3306,7 @@
     <x v="0"/>
     <x v="3"/>
     <x v="0"/>
-    <x v="6"/>
+    <n v="7"/>
     <n v="9.6152244606891379"/>
     <n v="9.018713248970311"/>
     <n v="1.0661414988204589"/>
@@ -3242,7 +3315,7 @@
     <x v="1"/>
     <x v="0"/>
     <x v="0"/>
-    <x v="6"/>
+    <n v="7"/>
     <n v="9.6338673861609294"/>
     <n v="9.0947451568496831"/>
     <n v="1.0592784316672368"/>
@@ -3251,7 +3324,7 @@
     <x v="1"/>
     <x v="1"/>
     <x v="0"/>
-    <x v="6"/>
+    <n v="7"/>
     <n v="9.6268022552766723"/>
     <n v="9.1126546408629316"/>
     <n v="1.0564212772980774"/>
@@ -3260,7 +3333,7 @@
     <x v="1"/>
     <x v="2"/>
     <x v="0"/>
-    <x v="6"/>
+    <n v="7"/>
     <n v="9.6209972445783905"/>
     <n v="9.0892006707668784"/>
     <n v="1.058508618422509"/>
@@ -3269,7 +3342,7 @@
     <x v="1"/>
     <x v="3"/>
     <x v="0"/>
-    <x v="6"/>
+    <n v="7"/>
     <n v="9.6152244606891379"/>
     <n v="9.018713248970311"/>
     <n v="1.0661414988204589"/>
@@ -3278,7 +3351,7 @@
     <x v="2"/>
     <x v="0"/>
     <x v="0"/>
-    <x v="6"/>
+    <n v="7"/>
     <n v="9.6225958817934654"/>
     <n v="9.0910646070264995"/>
     <n v="1.0584674400351466"/>
@@ -3287,7 +3360,7 @@
     <x v="2"/>
     <x v="1"/>
     <x v="0"/>
-    <x v="6"/>
+    <n v="7"/>
     <n v="9.6063334643967124"/>
     <n v="9.134989838322662"/>
     <n v="1.0515976081436558"/>
@@ -3296,7 +3369,7 @@
     <x v="2"/>
     <x v="2"/>
     <x v="0"/>
-    <x v="6"/>
+    <n v="7"/>
     <n v="9.637747815700612"/>
     <n v="9.1552404457313372"/>
     <n v="1.0527028615828704"/>
@@ -3305,7 +3378,7 @@
     <x v="2"/>
     <x v="3"/>
     <x v="0"/>
-    <x v="6"/>
+    <n v="7"/>
     <n v="9.6152244606891379"/>
     <n v="9.018713248970311"/>
     <n v="1.0661414988204589"/>
@@ -3314,7 +3387,7 @@
     <x v="3"/>
     <x v="0"/>
     <x v="0"/>
-    <x v="6"/>
+    <n v="7"/>
     <n v="9.6627578316815743"/>
     <n v="9.077364103720079"/>
     <n v="1.0644893959603967"/>
@@ -3323,7 +3396,7 @@
     <x v="3"/>
     <x v="1"/>
     <x v="0"/>
-    <x v="6"/>
+    <n v="7"/>
     <n v="9.5017302660547536"/>
     <n v="9.3177418734074564"/>
     <n v="1.0197460280770809"/>
@@ -3332,7 +3405,7 @@
     <x v="3"/>
     <x v="2"/>
     <x v="0"/>
-    <x v="6"/>
+    <n v="7"/>
     <n v="9.1625524914857035"/>
     <n v="9.4904559688884227"/>
     <n v="0.96544913347918671"/>
@@ -3341,7 +3414,7 @@
     <x v="3"/>
     <x v="3"/>
     <x v="0"/>
-    <x v="6"/>
+    <n v="7"/>
     <n v="9.6152244606891379"/>
     <n v="9.018713248970311"/>
     <n v="1.0661414988204589"/>
@@ -3350,7 +3423,7 @@
     <x v="4"/>
     <x v="0"/>
     <x v="0"/>
-    <x v="6"/>
+    <n v="7"/>
     <n v="9.5946890029210152"/>
     <n v="9.1269112193540369"/>
     <n v="1.0512525839601721"/>
@@ -3359,7 +3432,7 @@
     <x v="4"/>
     <x v="1"/>
     <x v="0"/>
-    <x v="6"/>
+    <n v="7"/>
     <n v="9.3010299956639813"/>
     <n v="9.5438907089047724"/>
     <n v="0.97455328014033171"/>
@@ -3368,7 +3441,7 @@
     <x v="4"/>
     <x v="2"/>
     <x v="0"/>
-    <x v="6"/>
+    <n v="7"/>
     <n v="8.7988475929627565"/>
     <n v="9.5486633678578876"/>
     <n v="0.92147426859563253"/>
@@ -3377,7 +3450,7 @@
     <x v="4"/>
     <x v="3"/>
     <x v="0"/>
-    <x v="6"/>
+    <n v="7"/>
     <n v="9.6152244606891379"/>
     <n v="9.018713248970311"/>
     <n v="1.0661414988204589"/>
@@ -3386,7 +3459,7 @@
     <x v="0"/>
     <x v="0"/>
     <x v="1"/>
-    <x v="5"/>
+    <n v="6"/>
     <n v="8.7852714699409482"/>
     <n v="9.287536162856906"/>
     <n v="0.94592056664881319"/>
@@ -3395,7 +3468,7 @@
     <x v="0"/>
     <x v="1"/>
     <x v="1"/>
-    <x v="5"/>
+    <n v="6"/>
     <n v="8.8600796517029785"/>
     <n v="9.3169865778948378"/>
     <n v="0.95095979559787058"/>
@@ -3404,7 +3477,7 @@
     <x v="0"/>
     <x v="2"/>
     <x v="1"/>
-    <x v="5"/>
+    <n v="6"/>
     <n v="9.0072602693789623"/>
     <n v="9.3769829329325809"/>
     <n v="0.96057125557356748"/>
@@ -3413,7 +3486,7 @@
     <x v="0"/>
     <x v="3"/>
     <x v="1"/>
-    <x v="5"/>
+    <n v="6"/>
     <n v="8.7921656121837657"/>
     <n v="9.3449207045687537"/>
     <n v="0.94084967546971854"/>
@@ -3422,7 +3495,7 @@
     <x v="1"/>
     <x v="0"/>
     <x v="1"/>
-    <x v="5"/>
+    <n v="6"/>
     <n v="8.8802112417116064"/>
     <n v="9.3004864478433742"/>
     <n v="0.95481148126082993"/>
@@ -3431,7 +3504,7 @@
     <x v="1"/>
     <x v="1"/>
     <x v="1"/>
-    <x v="5"/>
+    <n v="6"/>
     <n v="8.7311989989494769"/>
     <n v="9.2507350360502052"/>
     <n v="0.9438384047239391"/>
@@ -3440,7 +3513,7 @@
     <x v="1"/>
     <x v="2"/>
     <x v="1"/>
-    <x v="5"/>
+    <n v="6"/>
     <n v="8.9888618026444238"/>
     <n v="9.2612221167531601"/>
     <n v="0.97059132038135143"/>
@@ -3449,7 +3522,7 @@
     <x v="1"/>
     <x v="3"/>
     <x v="1"/>
-    <x v="5"/>
+    <n v="6"/>
     <n v="8.7921656121837657"/>
     <n v="9.3449207045687537"/>
     <n v="0.94084967546971854"/>
@@ -3458,7 +3531,7 @@
     <x v="2"/>
     <x v="0"/>
     <x v="1"/>
-    <x v="5"/>
+    <n v="6"/>
     <n v="8.8709695388645997"/>
     <n v="9.3061269530482189"/>
     <n v="0.95323968645827639"/>
@@ -3467,7 +3540,7 @@
     <x v="2"/>
     <x v="1"/>
     <x v="1"/>
-    <x v="5"/>
+    <n v="6"/>
     <n v="8.8613169612669065"/>
     <n v="9.360327678275862"/>
     <n v="0.94668875554783238"/>
@@ -3476,7 +3549,7 @@
     <x v="2"/>
     <x v="2"/>
     <x v="1"/>
-    <x v="5"/>
+    <n v="6"/>
     <n v="8.7032700902169786"/>
     <n v="9.4216786892189788"/>
     <n v="0.92374940573763575"/>
@@ -3485,7 +3558,7 @@
     <x v="2"/>
     <x v="3"/>
     <x v="1"/>
-    <x v="5"/>
+    <n v="6"/>
     <n v="8.7921656121837657"/>
     <n v="9.3449207045687537"/>
     <n v="0.94084967546971854"/>
@@ -3494,7 +3567,7 @@
     <x v="3"/>
     <x v="0"/>
     <x v="1"/>
-    <x v="5"/>
+    <n v="6"/>
     <n v="8.8890756251918219"/>
     <n v="9.3074486080165677"/>
     <n v="0.9550496596387974"/>
@@ -3503,7 +3576,7 @@
     <x v="3"/>
     <x v="1"/>
     <x v="1"/>
-    <x v="5"/>
+    <n v="6"/>
     <n v="8.854210450067356"/>
     <n v="9.2706023453416293"/>
     <n v="0.95508469894801329"/>
@@ -3512,7 +3585,7 @@
     <x v="3"/>
     <x v="2"/>
     <x v="1"/>
-    <x v="5"/>
+    <n v="6"/>
     <n v="8.8933757110727818"/>
     <n v="8.9542425094393252"/>
     <n v="0.9932024625977709"/>
@@ -3521,7 +3594,7 @@
     <x v="3"/>
     <x v="3"/>
     <x v="1"/>
-    <x v="5"/>
+    <n v="6"/>
     <n v="8.7921656121837657"/>
     <n v="9.3449207045687537"/>
     <n v="0.94084967546971854"/>
@@ -3530,7 +3603,7 @@
     <x v="4"/>
     <x v="0"/>
     <x v="1"/>
-    <x v="5"/>
+    <n v="6"/>
     <n v="8.7817405426972055"/>
     <n v="9.354040405234116"/>
     <n v="0.93881789710714991"/>
@@ -3539,7 +3612,7 @@
     <x v="4"/>
     <x v="1"/>
     <x v="1"/>
-    <x v="5"/>
+    <n v="6"/>
     <n v="8.8388034763602477"/>
     <n v="9.2428607132407912"/>
     <n v="0.95628439620411954"/>
@@ -3548,7 +3621,7 @@
     <x v="4"/>
     <x v="2"/>
     <x v="1"/>
-    <x v="5"/>
+    <n v="6"/>
     <n v="8.8129133566428557"/>
     <n v="9.1461280356782382"/>
     <n v="0.96356767828576839"/>
@@ -3557,7 +3630,7 @@
     <x v="4"/>
     <x v="3"/>
     <x v="1"/>
-    <x v="5"/>
+    <n v="6"/>
     <n v="8.7921656121837657"/>
     <n v="9.3449207045687537"/>
     <n v="0.94084967546971854"/>
@@ -3566,7 +3639,7 @@
     <x v="0"/>
     <x v="0"/>
     <x v="1"/>
-    <x v="6"/>
+    <n v="7"/>
     <n v="9.4699592101845287"/>
     <n v="9.1108374985353855"/>
     <n v="1.0394169813375416"/>
@@ -3575,7 +3648,7 @@
     <x v="0"/>
     <x v="1"/>
     <x v="1"/>
-    <x v="6"/>
+    <n v="7"/>
     <n v="9.4446508512531544"/>
     <n v="9.2139863568041047"/>
     <n v="1.0250341693070464"/>
@@ -3584,7 +3657,7 @@
     <x v="0"/>
     <x v="2"/>
     <x v="1"/>
-    <x v="6"/>
+    <n v="7"/>
     <n v="9.4357864677729388"/>
     <n v="9.2387776660994909"/>
     <n v="1.0213241197909055"/>
@@ -3593,7 +3666,7 @@
     <x v="0"/>
     <x v="3"/>
     <x v="1"/>
-    <x v="6"/>
+    <n v="7"/>
     <n v="9.3594998189393586"/>
     <n v="9.1901056208558032"/>
     <n v="1.0184322362627842"/>
@@ -3602,7 +3675,7 @@
     <x v="1"/>
     <x v="0"/>
     <x v="1"/>
-    <x v="6"/>
+    <n v="7"/>
     <n v="9.3965458000882904"/>
     <n v="9.2842768560247215"/>
     <n v="1.0120923735692691"/>
@@ -3611,7 +3684,7 @@
     <x v="1"/>
     <x v="1"/>
     <x v="1"/>
-    <x v="6"/>
+    <n v="7"/>
     <n v="9.3449207045687537"/>
     <n v="9.2898917983084051"/>
     <n v="1.0059235249941629"/>
@@ -3620,7 +3693,7 @@
     <x v="1"/>
     <x v="2"/>
     <x v="1"/>
-    <x v="6"/>
+    <n v="7"/>
     <n v="9.3966856244594776"/>
     <n v="9.2350581765755031"/>
     <n v="1.0175015083601679"/>
@@ -3629,7 +3702,7 @@
     <x v="1"/>
     <x v="3"/>
     <x v="1"/>
-    <x v="6"/>
+    <n v="7"/>
     <n v="9.3594998189393586"/>
     <n v="9.1901056208558032"/>
     <n v="1.0184322362627842"/>
@@ -3638,7 +3711,7 @@
     <x v="2"/>
     <x v="0"/>
     <x v="1"/>
-    <x v="6"/>
+    <n v="7"/>
     <n v="9.2274224300042551"/>
     <n v="9.3640144772102598"/>
     <n v="0.98541308884790424"/>
@@ -3647,7 +3720,7 @@
     <x v="2"/>
     <x v="1"/>
     <x v="1"/>
-    <x v="6"/>
+    <n v="7"/>
     <n v="9.0566373462321756"/>
     <n v="9.393553046518285"/>
     <n v="0.96413330519158702"/>
@@ -3656,7 +3729,7 @@
     <x v="2"/>
     <x v="2"/>
     <x v="1"/>
-    <x v="6"/>
+    <n v="7"/>
     <n v="9.096562299177231"/>
     <n v="9.4913616938342731"/>
     <n v="0.95840434624743998"/>
@@ -3665,7 +3738,7 @@
     <x v="2"/>
     <x v="3"/>
     <x v="1"/>
-    <x v="6"/>
+    <n v="7"/>
     <n v="9.3594998189393586"/>
     <n v="9.1901056208558032"/>
     <n v="1.0184322362627842"/>
@@ -3674,7 +3747,7 @@
     <x v="3"/>
     <x v="0"/>
     <x v="1"/>
-    <x v="6"/>
+    <n v="7"/>
     <n v="9.452628024374226"/>
     <n v="9.1450173056812591"/>
     <n v="1.0336369750226571"/>
@@ -3683,7 +3756,7 @@
     <x v="3"/>
     <x v="1"/>
     <x v="1"/>
-    <x v="6"/>
+    <n v="7"/>
     <n v="9.1162439331764933"/>
     <n v="9.2908041830160286"/>
     <n v="0.98121150264272727"/>
@@ -3692,7 +3765,7 @@
     <x v="3"/>
     <x v="2"/>
     <x v="1"/>
-    <x v="6"/>
+    <n v="7"/>
     <n v="8.6945830421822663"/>
     <n v="9.3844669710933921"/>
     <n v="0.92648661548533884"/>
@@ -3701,7 +3774,7 @@
     <x v="3"/>
     <x v="3"/>
     <x v="1"/>
-    <x v="6"/>
+    <n v="7"/>
     <n v="9.3594998189393586"/>
     <n v="9.1901056208558032"/>
     <n v="1.0184322362627842"/>
@@ -3710,7 +3783,7 @@
     <x v="4"/>
     <x v="0"/>
     <x v="1"/>
-    <x v="6"/>
+    <n v="7"/>
     <n v="9.0743013274030471"/>
     <n v="9.3333525680599507"/>
     <n v="0.9722445671297778"/>
@@ -3719,7 +3792,7 @@
     <x v="4"/>
     <x v="1"/>
     <x v="1"/>
-    <x v="6"/>
+    <n v="7"/>
     <n v="8.8459825513836812"/>
     <n v="9.3238870251344146"/>
     <n v="0.94874407288908091"/>
@@ -3728,7 +3801,7 @@
     <x v="4"/>
     <x v="2"/>
     <x v="1"/>
-    <x v="6"/>
+    <n v="7"/>
     <n v="8.8802112417116064"/>
     <n v="9.1928031367991565"/>
     <n v="0.96599601988252826"/>
@@ -3737,7 +3810,7 @@
     <x v="4"/>
     <x v="3"/>
     <x v="1"/>
-    <x v="6"/>
+    <n v="7"/>
     <n v="9.3594998189393586"/>
     <n v="9.1901056208558032"/>
     <n v="1.0184322362627842"/>
@@ -3746,7 +3819,7 @@
     <x v="0"/>
     <x v="0"/>
     <x v="2"/>
-    <x v="5"/>
+    <n v="6"/>
     <n v="8.6020599913279625"/>
     <n v="9.116498055196077"/>
     <n v="0.94357064952425418"/>
@@ -3755,7 +3828,7 @@
     <x v="0"/>
     <x v="1"/>
     <x v="2"/>
-    <x v="5"/>
+    <n v="6"/>
     <n v="8.8419735653757563"/>
     <n v="9.2764557251082547"/>
     <n v="0.95316291344370885"/>
@@ -3764,7 +3837,7 @@
     <x v="0"/>
     <x v="2"/>
     <x v="2"/>
-    <x v="5"/>
+    <n v="6"/>
     <n v="8.88616085336146"/>
     <n v="9.4006332352448112"/>
     <n v="0.94527258228153255"/>
@@ -3773,7 +3846,7 @@
     <x v="0"/>
     <x v="3"/>
     <x v="2"/>
-    <x v="5"/>
+    <n v="6"/>
     <n v="8.8388034763602477"/>
     <n v="9.2558748556724915"/>
     <n v="0.9549398208364237"/>
@@ -3782,7 +3855,7 @@
     <x v="1"/>
     <x v="0"/>
     <x v="2"/>
-    <x v="5"/>
+    <n v="6"/>
     <n v="8.759256969938944"/>
     <n v="9.2505981210135442"/>
     <n v="0.946885472198984"/>
@@ -3791,7 +3864,7 @@
     <x v="1"/>
     <x v="1"/>
     <x v="2"/>
-    <x v="5"/>
+    <n v="6"/>
     <n v="8.8116246451989504"/>
     <n v="9.0877559066817248"/>
     <n v="0.9696150221992923"/>
@@ -3800,7 +3873,7 @@
     <x v="1"/>
     <x v="2"/>
     <x v="2"/>
-    <x v="5"/>
+    <n v="6"/>
     <n v="9.2131742868937536"/>
     <n v="9.1944057067367631"/>
     <n v="1.0020413043273955"/>
@@ -3809,7 +3882,7 @@
     <x v="1"/>
     <x v="3"/>
     <x v="2"/>
-    <x v="5"/>
+    <n v="6"/>
     <n v="8.8388034763602477"/>
     <n v="9.2558748556724915"/>
     <n v="0.9549398208364237"/>
@@ -3818,7 +3891,7 @@
     <x v="2"/>
     <x v="0"/>
     <x v="2"/>
-    <x v="5"/>
+    <n v="6"/>
     <n v="8.7670130530280677"/>
     <n v="9.2558748556724915"/>
     <n v="0.94718362010428181"/>
@@ -3827,7 +3900,7 @@
     <x v="2"/>
     <x v="1"/>
     <x v="2"/>
-    <x v="5"/>
+    <n v="6"/>
     <n v="8.7763341080560977"/>
     <n v="9.3675598170409362"/>
     <n v="0.93688583574248285"/>
@@ -3836,7 +3909,7 @@
     <x v="2"/>
     <x v="2"/>
     <x v="2"/>
-    <x v="5"/>
+    <n v="6"/>
     <n v="8.5909217939723863"/>
     <n v="9.4555255101640636"/>
     <n v="0.90856100855925082"/>
@@ -3845,7 +3918,7 @@
     <x v="2"/>
     <x v="3"/>
     <x v="2"/>
-    <x v="5"/>
+    <n v="6"/>
     <n v="8.8388034763602477"/>
     <n v="9.2558748556724915"/>
     <n v="0.9549398208364237"/>
@@ -3854,7 +3927,7 @@
     <x v="3"/>
     <x v="0"/>
     <x v="2"/>
-    <x v="5"/>
+    <n v="6"/>
     <n v="8.7585979489749874"/>
     <n v="9.2685315713908096"/>
     <n v="0.94498226407408104"/>
@@ -3863,7 +3936,7 @@
     <x v="3"/>
     <x v="1"/>
     <x v="2"/>
-    <x v="5"/>
+    <n v="6"/>
     <n v="8.6855339311358684"/>
     <n v="9.2951979735920069"/>
     <n v="0.93441085986675954"/>
@@ -3872,7 +3945,7 @@
     <x v="3"/>
     <x v="2"/>
     <x v="2"/>
-    <x v="5"/>
+    <n v="6"/>
     <n v="8.6505149978319906"/>
     <n v="9.1147129239603473"/>
     <n v="0.94907158020214832"/>
@@ -3881,7 +3954,7 @@
     <x v="3"/>
     <x v="3"/>
     <x v="2"/>
-    <x v="5"/>
+    <n v="6"/>
     <n v="8.8388034763602477"/>
     <n v="9.2558748556724915"/>
     <n v="0.9549398208364237"/>
@@ -3890,7 +3963,7 @@
     <x v="4"/>
     <x v="0"/>
     <x v="2"/>
-    <x v="5"/>
+    <n v="6"/>
     <n v="8.5730640178391191"/>
     <n v="9.3354011421304719"/>
     <n v="0.91833911444351957"/>
@@ -3899,7 +3972,7 @@
     <x v="4"/>
     <x v="1"/>
     <x v="2"/>
-    <x v="5"/>
+    <n v="6"/>
     <n v="8.5791812460476251"/>
     <n v="9.2618732334057832"/>
     <n v="0.92629007435603627"/>
@@ -3908,7 +3981,7 @@
     <x v="4"/>
     <x v="2"/>
     <x v="2"/>
-    <x v="5"/>
+    <n v="6"/>
     <n v="8.4097719677709346"/>
     <n v="9.1673173347481764"/>
     <n v="0.9173645528658847"/>
@@ -3917,7 +3990,7 @@
     <x v="4"/>
     <x v="3"/>
     <x v="2"/>
-    <x v="5"/>
+    <n v="6"/>
     <n v="8.8388034763602477"/>
     <n v="9.2558748556724915"/>
     <n v="0.9549398208364237"/>
@@ -3926,7 +3999,7 @@
     <x v="0"/>
     <x v="0"/>
     <x v="2"/>
-    <x v="6"/>
+    <n v="7"/>
     <n v="9.4479321756236487"/>
     <n v="8.8996702747267911"/>
     <n v="1.0616047430941129"/>
@@ -3935,7 +4008,7 @@
     <x v="0"/>
     <x v="1"/>
     <x v="2"/>
-    <x v="6"/>
+    <n v="7"/>
     <n v="9.5230719203746137"/>
     <n v="8.9697596263093082"/>
     <n v="1.0616864126929755"/>
@@ -3944,7 +4017,7 @@
     <x v="0"/>
     <x v="2"/>
     <x v="2"/>
-    <x v="6"/>
+    <n v="7"/>
     <n v="9.6227563339070752"/>
     <n v="8.968256871239447"/>
     <n v="1.0729795624795897"/>
@@ -3953,7 +4026,7 @@
     <x v="0"/>
     <x v="3"/>
     <x v="2"/>
-    <x v="6"/>
+    <n v="7"/>
     <n v="9.5114203054382642"/>
     <n v="8.9259348003648835"/>
     <n v="1.065593746556321"/>
@@ -3962,7 +4035,7 @@
     <x v="1"/>
     <x v="0"/>
     <x v="2"/>
-    <x v="6"/>
+    <n v="7"/>
     <n v="9.5128167555303484"/>
     <n v="8.9722413360750846"/>
     <n v="1.0602497635993973"/>
@@ -3971,7 +4044,7 @@
     <x v="1"/>
     <x v="1"/>
     <x v="2"/>
-    <x v="6"/>
+    <n v="7"/>
     <n v="9.5145294750422504"/>
     <n v="9.1090050214921821"/>
     <n v="1.0445190723458002"/>
@@ -3980,7 +4053,7 @@
     <x v="1"/>
     <x v="2"/>
     <x v="2"/>
-    <x v="6"/>
+    <n v="7"/>
     <n v="9.5299709440309783"/>
     <n v="8.9978175972987753"/>
     <n v="1.0591424910516034"/>
@@ -3989,7 +4062,7 @@
     <x v="1"/>
     <x v="3"/>
     <x v="2"/>
-    <x v="6"/>
+    <n v="7"/>
     <n v="9.5114203054382642"/>
     <n v="8.9259348003648835"/>
     <n v="1.065593746556321"/>
@@ -3998,7 +4071,7 @@
     <x v="2"/>
     <x v="0"/>
     <x v="2"/>
-    <x v="6"/>
+    <n v="7"/>
     <n v="9.4605830253188685"/>
     <n v="8.9911356165197844"/>
     <n v="1.0522122486882024"/>
@@ -4007,7 +4080,7 @@
     <x v="2"/>
     <x v="1"/>
     <x v="2"/>
-    <x v="6"/>
+    <n v="7"/>
     <n v="9.2540627680415994"/>
     <n v="9.2145530041663477"/>
     <n v="1.0042877569706732"/>
@@ -4016,7 +4089,7 @@
     <x v="2"/>
     <x v="2"/>
     <x v="2"/>
-    <x v="6"/>
+    <n v="7"/>
     <n v="8.8406206186877938"/>
     <n v="9.4805918549062191"/>
     <n v="0.93249669999376261"/>
@@ -4025,7 +4098,7 @@
     <x v="2"/>
     <x v="3"/>
     <x v="2"/>
-    <x v="6"/>
+    <n v="7"/>
     <n v="9.5114203054382642"/>
     <n v="8.9259348003648835"/>
     <n v="1.065593746556321"/>
@@ -4034,7 +4107,7 @@
     <x v="3"/>
     <x v="0"/>
     <x v="2"/>
-    <x v="6"/>
+    <n v="7"/>
     <n v="9.4675015757268284"/>
     <n v="8.9259348003648835"/>
     <n v="1.0606733958374652"/>
@@ -4043,7 +4116,7 @@
     <x v="3"/>
     <x v="1"/>
     <x v="2"/>
-    <x v="6"/>
+    <n v="7"/>
     <n v="9.1746387637339772"/>
     <n v="9.2354990848304368"/>
     <n v="0.99341017517976649"/>
@@ -4052,7 +4125,7 @@
     <x v="3"/>
     <x v="2"/>
     <x v="2"/>
-    <x v="6"/>
+    <n v="7"/>
     <n v="8.6760912590556813"/>
     <n v="9.1461280356782382"/>
     <n v="0.94860811320495575"/>
@@ -4061,7 +4134,7 @@
     <x v="3"/>
     <x v="3"/>
     <x v="2"/>
-    <x v="6"/>
+    <n v="7"/>
     <n v="9.5114203054382642"/>
     <n v="8.9259348003648835"/>
     <n v="1.065593746556321"/>
@@ -4070,7 +4143,7 @@
     <x v="4"/>
     <x v="0"/>
     <x v="2"/>
-    <x v="6"/>
+    <n v="7"/>
     <n v="9.1564059131060453"/>
     <n v="9.2296962438796157"/>
     <n v="0.99205929113624181"/>
@@ -4079,7 +4152,7 @@
     <x v="4"/>
     <x v="1"/>
     <x v="2"/>
-    <x v="6"/>
+    <n v="7"/>
     <n v="8.7392832477969229"/>
     <n v="9.1522452638867442"/>
     <n v="0.95487861129341656"/>
@@ -4088,7 +4161,7 @@
     <x v="4"/>
     <x v="2"/>
     <x v="2"/>
-    <x v="6"/>
+    <n v="7"/>
     <n v="8.1901056208558032"/>
     <n v="9.2241985517288843"/>
     <n v="0.88789346574947026"/>
@@ -4097,7 +4170,7 @@
     <x v="4"/>
     <x v="3"/>
     <x v="2"/>
-    <x v="6"/>
+    <n v="7"/>
     <n v="9.5114203054382642"/>
     <n v="8.9259348003648835"/>
     <n v="1.065593746556321"/>
@@ -4106,7 +4179,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable1" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable1" cacheId="6" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A3:G82" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="7">
     <pivotField axis="axisRow" showAll="0">
@@ -4136,18 +4209,7 @@
         <item t="default"/>
       </items>
     </pivotField>
-    <pivotField showAll="0">
-      <items count="8">
-        <item x="0"/>
-        <item x="1"/>
-        <item x="2"/>
-        <item x="3"/>
-        <item x="4"/>
-        <item x="5"/>
-        <item x="6"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
+    <pivotField showAll="0"/>
     <pivotField dataField="1" numFmtId="2" showAll="0"/>
     <pivotField dataField="1" numFmtId="2" showAll="0"/>
     <pivotField dataField="1" numFmtId="2" showAll="0"/>
@@ -4427,27 +4489,252 @@
     <dataField name="Average of Ratio" fld="6" subtotal="average" baseField="2" baseItem="0"/>
     <dataField name="StdDev of Ratio" fld="6" subtotal="stdDev" baseField="2" baseItem="0"/>
   </dataFields>
-  <formats count="7">
-    <format dxfId="6">
+  <formats count="22">
+    <format dxfId="28">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
-    <format dxfId="5">
+    <format dxfId="27">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
-    <format dxfId="4">
+    <format dxfId="26">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
-    <format dxfId="3">
+    <format dxfId="25">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
-    <format dxfId="2">
+    <format dxfId="24">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
-    <format dxfId="1">
+    <format dxfId="23">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
+    <format dxfId="22">
+      <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
+    </format>
+    <format dxfId="14">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="4"/>
+          </reference>
+          <reference field="2" count="1">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="13">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="4"/>
+          </reference>
+          <reference field="2" count="1">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="12">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="4"/>
+          </reference>
+          <reference field="2" count="1">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="11">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="4"/>
+          </reference>
+          <reference field="2" count="1">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="10">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="4"/>
+          </reference>
+          <reference field="2" count="1">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="9">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="3">
+          <reference field="4294967294" count="2" selected="0">
+            <x v="4"/>
+            <x v="5"/>
+          </reference>
+          <reference field="0" count="1">
+            <x v="0"/>
+          </reference>
+          <reference field="2" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="8">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="4">
+          <reference field="4294967294" count="2" selected="0">
+            <x v="4"/>
+            <x v="5"/>
+          </reference>
+          <reference field="0" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="1" count="0"/>
+          <reference field="2" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="7">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="3">
+          <reference field="4294967294" count="2" selected="0">
+            <x v="4"/>
+            <x v="5"/>
+          </reference>
+          <reference field="0" count="1">
+            <x v="0"/>
+          </reference>
+          <reference field="2" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="6">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="4">
+          <reference field="4294967294" count="2" selected="0">
+            <x v="4"/>
+            <x v="5"/>
+          </reference>
+          <reference field="0" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="1" count="0"/>
+          <reference field="2" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="5">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="3">
+          <reference field="4294967294" count="2" selected="0">
+            <x v="4"/>
+            <x v="5"/>
+          </reference>
+          <reference field="0" count="1">
+            <x v="0"/>
+          </reference>
+          <reference field="2" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="4">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="4">
+          <reference field="4294967294" count="2" selected="0">
+            <x v="4"/>
+            <x v="5"/>
+          </reference>
+          <reference field="0" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="1" count="0"/>
+          <reference field="2" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="3">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="3">
+          <reference field="4294967294" count="2" selected="0">
+            <x v="4"/>
+            <x v="5"/>
+          </reference>
+          <reference field="0" count="1">
+            <x v="0"/>
+          </reference>
+          <reference field="2" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="2">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="4">
+          <reference field="4294967294" count="2" selected="0">
+            <x v="4"/>
+            <x v="5"/>
+          </reference>
+          <reference field="0" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="1" count="0"/>
+          <reference field="2" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="1">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="3">
+          <reference field="4294967294" count="2" selected="0">
+            <x v="4"/>
+            <x v="5"/>
+          </reference>
+          <reference field="0" count="1">
+            <x v="0"/>
+          </reference>
+          <reference field="2" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
     <format dxfId="0">
-      <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="4">
+          <reference field="4294967294" count="2" selected="0">
+            <x v="4"/>
+            <x v="5"/>
+          </reference>
+          <reference field="0" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="1" count="0"/>
+          <reference field="2" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
     </format>
   </formats>
   <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
@@ -4724,8 +5011,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V421"/>
   <sheetViews>
-    <sheetView topLeftCell="A394" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="A301" sqref="A301:G301"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="J18" sqref="J18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4788,13 +5075,13 @@
       <c r="D2">
         <v>1</v>
       </c>
-      <c r="E2" s="13">
+      <c r="E2" s="37">
         <v>9.4240098632701716</v>
       </c>
-      <c r="F2" s="13">
+      <c r="F2" s="37">
         <v>9.7959954431166096</v>
       </c>
-      <c r="G2" s="17">
+      <c r="G2" s="35">
         <f>E2/F2</f>
         <v>0.96202677083646226</v>
       </c>
@@ -4822,13 +5109,13 @@
       <c r="D3">
         <v>1</v>
       </c>
-      <c r="E3" s="13">
+      <c r="E3" s="37">
         <v>9.5088065209152948</v>
       </c>
-      <c r="F3" s="13">
+      <c r="F3" s="37">
         <v>9.71093626081195</v>
       </c>
-      <c r="G3" s="17">
+      <c r="G3" s="35">
         <f t="shared" ref="G3:G61" si="0">E3/F3</f>
         <v>0.97918534995308937</v>
       </c>
@@ -4858,13 +5145,13 @@
       <c r="D4">
         <v>1</v>
       </c>
-      <c r="E4" s="14">
+      <c r="E4" s="38">
         <v>9.3935803223956835</v>
       </c>
-      <c r="F4" s="14">
+      <c r="F4" s="38">
         <v>9.7518996874222506</v>
       </c>
-      <c r="G4" s="17">
+      <c r="G4" s="35">
         <f t="shared" si="0"/>
         <v>0.96325645499730495</v>
       </c>
@@ -4896,13 +5183,13 @@
       <c r="D5">
         <v>1</v>
       </c>
-      <c r="E5" s="13">
+      <c r="E5" s="37">
         <v>9.251318383953441</v>
       </c>
-      <c r="F5" s="13">
+      <c r="F5" s="37">
         <v>9.7589590804382453</v>
       </c>
-      <c r="G5" s="17">
+      <c r="G5" s="35">
         <f t="shared" si="0"/>
         <v>0.94798208576339194</v>
       </c>
@@ -4934,13 +5221,13 @@
       <c r="D6">
         <v>1</v>
       </c>
-      <c r="E6" s="13">
+      <c r="E6" s="37">
         <v>9.3311163808053248</v>
       </c>
-      <c r="F6" s="13">
+      <c r="F6" s="37">
         <v>9.8003202707418868</v>
       </c>
-      <c r="G6" s="17">
+      <c r="G6" s="35">
         <f t="shared" si="0"/>
         <v>0.95212361668043288</v>
       </c>
@@ -4972,13 +5259,13 @@
       <c r="D7">
         <v>1</v>
       </c>
-      <c r="E7" s="13">
+      <c r="E7" s="37">
         <v>9.4477477055885029</v>
       </c>
-      <c r="F7" s="13">
+      <c r="F7" s="37">
         <v>9.7634354841728648</v>
       </c>
-      <c r="G7" s="17">
+      <c r="G7" s="35">
         <f t="shared" si="0"/>
         <v>0.96766632205476122</v>
       </c>
@@ -5010,13 +5297,13 @@
       <c r="D8">
         <v>1</v>
       </c>
-      <c r="E8" s="14">
+      <c r="E8" s="38">
         <v>9.6001217007287352</v>
       </c>
-      <c r="F8" s="14">
+      <c r="F8" s="38">
         <v>9.8325254861957845</v>
       </c>
-      <c r="G8" s="17">
+      <c r="G8" s="35">
         <f t="shared" si="0"/>
         <v>0.9763637749230013</v>
       </c>
@@ -5048,13 +5335,13 @@
       <c r="D9">
         <v>1</v>
       </c>
-      <c r="E9" s="13">
+      <c r="E9" s="37">
         <v>9.251318383953441</v>
       </c>
-      <c r="F9" s="13">
+      <c r="F9" s="37">
         <v>9.7589590804382453</v>
       </c>
-      <c r="G9" s="17">
+      <c r="G9" s="35">
         <f t="shared" si="0"/>
         <v>0.94798208576339194</v>
       </c>
@@ -5086,13 +5373,13 @@
       <c r="D10">
         <v>1</v>
       </c>
-      <c r="E10" s="13">
+      <c r="E10" s="37">
         <v>9.2684762698640881</v>
       </c>
-      <c r="F10" s="13">
+      <c r="F10" s="37">
         <v>9.8419553938948123</v>
       </c>
-      <c r="G10" s="17">
+      <c r="G10" s="35">
         <f t="shared" si="0"/>
         <v>0.94173118033165781</v>
       </c>
@@ -5124,13 +5411,13 @@
       <c r="D11">
         <v>1</v>
       </c>
-      <c r="E11" s="13">
+      <c r="E11" s="37">
         <v>9.3866328741010463</v>
       </c>
-      <c r="F11" s="13">
+      <c r="F11" s="37">
         <v>9.7635026093269897</v>
       </c>
-      <c r="G11" s="17">
+      <c r="G11" s="35">
         <f t="shared" si="0"/>
         <v>0.96140015009921509</v>
       </c>
@@ -5162,13 +5449,13 @@
       <c r="D12">
         <v>1</v>
       </c>
-      <c r="E12" s="14">
+      <c r="E12" s="38">
         <v>9.3753785433333565</v>
       </c>
-      <c r="F12" s="14">
+      <c r="F12" s="38">
         <v>9.8360597390209517</v>
       </c>
-      <c r="G12" s="17">
+      <c r="G12" s="35">
         <f t="shared" si="0"/>
         <v>0.95316405065536436</v>
       </c>
@@ -5200,13 +5487,13 @@
       <c r="D13">
         <v>1</v>
       </c>
-      <c r="E13" s="13">
+      <c r="E13" s="37">
         <v>9.251318383953441</v>
       </c>
-      <c r="F13" s="13">
+      <c r="F13" s="37">
         <v>9.7589590804382453</v>
       </c>
-      <c r="G13" s="17">
+      <c r="G13" s="35">
         <f t="shared" si="0"/>
         <v>0.94798208576339194</v>
       </c>
@@ -5238,13 +5525,13 @@
       <c r="D14">
         <v>1</v>
       </c>
-      <c r="E14" s="13">
+      <c r="E14" s="37">
         <v>9.2926549660873778</v>
       </c>
-      <c r="F14" s="13">
+      <c r="F14" s="37">
         <v>9.7513091228089159</v>
       </c>
-      <c r="G14" s="17">
+      <c r="G14" s="35">
         <f t="shared" si="0"/>
         <v>0.95296486338960196</v>
       </c>
@@ -5276,13 +5563,13 @@
       <c r="D15">
         <v>1</v>
       </c>
-      <c r="E15" s="13">
+      <c r="E15" s="37">
         <v>9.1502446512516684</v>
       </c>
-      <c r="F15" s="13">
+      <c r="F15" s="37">
         <v>9.8269044061909163</v>
       </c>
-      <c r="G15" s="17">
+      <c r="G15" s="35">
         <f t="shared" si="0"/>
         <v>0.93114212503044658</v>
       </c>
@@ -5314,13 +5601,13 @@
       <c r="D16">
         <v>1</v>
       </c>
-      <c r="E16" s="14">
+      <c r="E16" s="38">
         <v>8.7388714951670927</v>
       </c>
-      <c r="F16" s="14">
+      <c r="F16" s="38">
         <v>9.8245504015026643</v>
       </c>
-      <c r="G16" s="17">
+      <c r="G16" s="35">
         <f t="shared" si="0"/>
         <v>0.88949327328306882</v>
       </c>
@@ -5352,13 +5639,13 @@
       <c r="D17">
         <v>1</v>
       </c>
-      <c r="E17" s="13">
+      <c r="E17" s="37">
         <v>9.251318383953441</v>
       </c>
-      <c r="F17" s="13">
+      <c r="F17" s="37">
         <v>9.7589590804382453</v>
       </c>
-      <c r="G17" s="17">
+      <c r="G17" s="35">
         <f t="shared" si="0"/>
         <v>0.94798208576339194</v>
       </c>
@@ -5390,13 +5677,13 @@
       <c r="D18">
         <v>1</v>
       </c>
-      <c r="E18" s="13">
+      <c r="E18" s="37">
         <v>9.2630141721297949</v>
       </c>
-      <c r="F18" s="13">
+      <c r="F18" s="37">
         <v>9.8023631994928646</v>
       </c>
-      <c r="G18" s="17">
+      <c r="G18" s="35">
         <f t="shared" si="0"/>
         <v>0.94497765320601734</v>
       </c>
@@ -5428,13 +5715,13 @@
       <c r="D19">
         <v>1</v>
       </c>
-      <c r="E19" s="13">
+      <c r="E19" s="37">
         <v>8.9744354014395178</v>
       </c>
-      <c r="F19" s="13">
+      <c r="F19" s="37">
         <v>9.8607583110976247</v>
       </c>
-      <c r="G19" s="17">
+      <c r="G19" s="35">
         <f t="shared" si="0"/>
         <v>0.91011615114218858</v>
       </c>
@@ -5466,13 +5753,13 @@
       <c r="D20">
         <v>1</v>
       </c>
-      <c r="E20" s="14">
+      <c r="E20" s="38">
         <v>8.5061713132926293</v>
       </c>
-      <c r="F20" s="14">
+      <c r="F20" s="38">
         <v>9.8690321730233617</v>
       </c>
-      <c r="G20" s="17">
+      <c r="G20" s="35">
         <f t="shared" si="0"/>
         <v>0.86190531798487169</v>
       </c>
@@ -5504,13 +5791,13 @@
       <c r="D21" s="5">
         <v>1</v>
       </c>
-      <c r="E21" s="14">
+      <c r="E21" s="38">
         <v>9.251318383953441</v>
       </c>
-      <c r="F21" s="14">
+      <c r="F21" s="38">
         <v>9.7589590804382453</v>
       </c>
-      <c r="G21" s="17">
+      <c r="G21" s="35">
         <f t="shared" si="0"/>
         <v>0.94798208576339194</v>
       </c>
@@ -7931,8 +8218,8 @@
       <c r="C86">
         <v>0</v>
       </c>
-      <c r="D86">
-        <v>2</v>
+      <c r="D86" s="33">
+        <v>3</v>
       </c>
       <c r="E86" s="17">
         <v>9.7192498325707817</v>
@@ -17217,8 +17504,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A3:G82"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H17" sqref="H17"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J18" sqref="J18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -17271,7 +17558,7 @@
       <c r="E4" s="17">
         <v>0.31913138175340128</v>
       </c>
-      <c r="F4" s="17">
+      <c r="F4" s="34">
         <v>1.0147485494345407</v>
       </c>
       <c r="G4" s="17">
@@ -17294,10 +17581,10 @@
       <c r="E5" s="17">
         <v>0.31438804708612866</v>
       </c>
-      <c r="F5" s="17">
+      <c r="F5" s="36">
         <v>1.0446240246558725</v>
       </c>
-      <c r="G5" s="17">
+      <c r="G5" s="36">
         <v>5.3809435426299047E-2</v>
       </c>
     </row>
@@ -17317,10 +17604,10 @@
       <c r="E6" s="17">
         <v>0.29230963540180921</v>
       </c>
-      <c r="F6" s="17">
+      <c r="F6" s="36">
         <v>1.03377448102944</v>
       </c>
-      <c r="G6" s="17">
+      <c r="G6" s="36">
         <v>5.3557779338223484E-2</v>
       </c>
     </row>
@@ -17340,10 +17627,10 @@
       <c r="E7" s="17">
         <v>0.35587502580188829</v>
       </c>
-      <c r="F7" s="17">
+      <c r="F7" s="36">
         <v>1.0476133885910583</v>
       </c>
-      <c r="G7" s="17">
+      <c r="G7" s="36">
         <v>5.8900606664506382E-2</v>
       </c>
     </row>
@@ -17363,10 +17650,10 @@
       <c r="E8" s="17">
         <v>0.34097871996381529</v>
       </c>
-      <c r="F8" s="17">
+      <c r="F8" s="36">
         <v>1.0513620558257304</v>
       </c>
-      <c r="G8" s="17">
+      <c r="G8" s="36">
         <v>5.6011834474042579E-2</v>
       </c>
     </row>
@@ -17386,10 +17673,10 @@
       <c r="E9" s="17">
         <v>0.33753211269207889</v>
       </c>
-      <c r="F9" s="17">
+      <c r="F9" s="36">
         <v>1.0457461731772626</v>
       </c>
-      <c r="G9" s="17">
+      <c r="G9" s="36">
         <v>5.789915545419394E-2</v>
       </c>
     </row>

</xml_diff>